<commit_message>
Updated project git repository, added post 529 for the OpenGL Samples Pack 4.3.1.0 release, updated status
</commit_message>
<xml_diff>
--- a/doc/OpenGL status.xlsx
+++ b/doc/OpenGL status.xlsx
@@ -305,6 +305,20 @@
           </rPr>
           <t xml:space="preserve">Zoming and rotating the quad shows tessellated triangle disappearing
 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G87" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>One of the two quad is not displayed</t>
         </r>
       </text>
     </comment>
@@ -1056,7 +1070,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1393" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="161">
   <si>
     <t>gl-430-texture-view</t>
   </si>
@@ -1536,6 +1550,9 @@
   </si>
   <si>
     <t>4.3.1.0</t>
+  </si>
+  <si>
+    <t>15.31.64.2885</t>
   </si>
 </sst>
 </file>
@@ -1682,7 +1699,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1711,12 +1728,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1725,6 +1736,16 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma 2" xfId="3"/>
@@ -2039,10 +2060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F195"/>
+  <dimension ref="A1:G195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2051,27 +2072,28 @@
     <col min="2" max="3" width="12.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="7" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="26"/>
+      <c r="F1" s="26" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="26"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>149</v>
       </c>
@@ -2090,8 +2112,11 @@
       <c r="F2" s="17">
         <v>41250</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="24">
+        <v>41259</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>148</v>
       </c>
@@ -2110,9 +2135,12 @@
       <c r="F3" s="2" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="G3" s="23" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
         <v>157</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -2130,8 +2158,11 @@
       <c r="F4" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G4" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -2139,7 +2170,7 @@
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>128</v>
       </c>
@@ -2148,8 +2179,9 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>129</v>
       </c>
@@ -2163,7 +2195,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>130</v>
       </c>
@@ -2177,7 +2209,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>132</v>
       </c>
@@ -2191,7 +2223,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>133</v>
       </c>
@@ -2205,7 +2237,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>134</v>
       </c>
@@ -2219,7 +2251,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>135</v>
       </c>
@@ -2233,7 +2265,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>136</v>
       </c>
@@ -2247,7 +2279,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>137</v>
       </c>
@@ -2261,7 +2293,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>138</v>
       </c>
@@ -2275,7 +2307,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
@@ -2289,7 +2321,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>0</v>
       </c>
@@ -2303,7 +2335,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>1</v>
       </c>
@@ -2317,7 +2349,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>2</v>
       </c>
@@ -2331,7 +2363,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>3</v>
       </c>
@@ -2345,21 +2377,22 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="23" t="s">
+      <c r="B21" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="21" t="s">
         <v>6</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="15"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>6</v>
       </c>
@@ -2383,8 +2416,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="10">
+        <f>COUNTIF(G7:G21,"pass")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>143</v>
       </c>
@@ -2408,8 +2445,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="5">
+        <f>COUNTIF(G7:G21,"Ok")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>140</v>
       </c>
@@ -2433,8 +2474,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="11">
+        <f>COUNTIF(G7:G21,"workaround")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -2458,8 +2503,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" s="12">
+        <f>COUNTIF(G7:G21,"Fail")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>145</v>
       </c>
@@ -2483,8 +2532,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="2">
+        <f>COUNT(G7:G21,"Untested")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>139</v>
       </c>
@@ -2508,8 +2561,12 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G27" s="2">
+        <f t="shared" ref="G27" si="6">G22+G25+G24+G26+G23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="18" t="s">
         <v>8</v>
       </c>
@@ -2522,27 +2579,32 @@
         <v>0.8</v>
       </c>
       <c r="D28" s="6" t="e">
-        <f t="shared" ref="D28:F28" si="6">(D22+D23)/D27</f>
+        <f t="shared" ref="D28:F28" si="7">(D22+D23)/D27</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E28" s="6" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F28" s="6" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G28" s="6" t="e">
+        <f t="shared" ref="G28" si="8">(G22+G23)/G27</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>102</v>
       </c>
@@ -2551,8 +2613,9 @@
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>94</v>
       </c>
@@ -2569,8 +2632,9 @@
         <v>6</v>
       </c>
       <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>97</v>
       </c>
@@ -2587,8 +2651,9 @@
         <v>6</v>
       </c>
       <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>98</v>
       </c>
@@ -2605,8 +2670,9 @@
         <v>6</v>
       </c>
       <c r="F33" s="2"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>99</v>
       </c>
@@ -2623,8 +2689,9 @@
         <v>6</v>
       </c>
       <c r="F34" s="2"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>100</v>
       </c>
@@ -2641,26 +2708,24 @@
         <v>6</v>
       </c>
       <c r="F35" s="2"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="B36" s="27"/>
       <c r="C36" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D36" s="27"/>
       <c r="E36" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F36" s="2"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>103</v>
       </c>
@@ -2677,8 +2742,9 @@
         <v>6</v>
       </c>
       <c r="F37" s="2"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>108</v>
       </c>
@@ -2695,8 +2761,9 @@
         <v>6</v>
       </c>
       <c r="F38" s="2"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38" s="2"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>109</v>
       </c>
@@ -2713,8 +2780,9 @@
         <v>6</v>
       </c>
       <c r="F39" s="2"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39" s="2"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>110</v>
       </c>
@@ -2731,8 +2799,9 @@
         <v>6</v>
       </c>
       <c r="F40" s="2"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>111</v>
       </c>
@@ -2749,8 +2818,9 @@
         <v>6</v>
       </c>
       <c r="F41" s="2"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41" s="2"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>112</v>
       </c>
@@ -2767,8 +2837,9 @@
         <v>6</v>
       </c>
       <c r="F42" s="2"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42" s="2"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>113</v>
       </c>
@@ -2785,8 +2856,9 @@
         <v>6</v>
       </c>
       <c r="F43" s="2"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43" s="2"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>115</v>
       </c>
@@ -2803,8 +2875,9 @@
         <v>6</v>
       </c>
       <c r="F44" s="2"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44" s="2"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>116</v>
       </c>
@@ -2821,8 +2894,9 @@
         <v>6</v>
       </c>
       <c r="F45" s="2"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>118</v>
       </c>
@@ -2839,8 +2913,9 @@
         <v>6</v>
       </c>
       <c r="F46" s="2"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46" s="2"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>120</v>
       </c>
@@ -2857,8 +2932,9 @@
         <v>6</v>
       </c>
       <c r="F47" s="2"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47" s="2"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>121</v>
       </c>
@@ -2875,8 +2951,9 @@
         <v>7</v>
       </c>
       <c r="F48" s="2"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48" s="2"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>122</v>
       </c>
@@ -2893,8 +2970,9 @@
         <v>6</v>
       </c>
       <c r="F49" s="2"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49" s="2"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>123</v>
       </c>
@@ -2911,8 +2989,9 @@
         <v>6</v>
       </c>
       <c r="F50" s="2"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50" s="2"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>124</v>
       </c>
@@ -2929,8 +3008,9 @@
         <v>6</v>
       </c>
       <c r="F51" s="2"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G51" s="2"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>126</v>
       </c>
@@ -2947,51 +3027,57 @@
         <v>140</v>
       </c>
       <c r="F52" s="2"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G52" s="2"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="B53" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C53" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D53" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="E53" s="23" t="s">
+      <c r="B53" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" s="21" t="s">
         <v>6</v>
       </c>
       <c r="F53" s="15"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G53" s="15"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B54" s="10">
         <f>COUNTIF(B31:B53,"pass")</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C54" s="10">
         <f>COUNTIF(C31:C53,"pass")</f>
         <v>21</v>
       </c>
       <c r="D54" s="10">
-        <f t="shared" ref="D54:F54" si="7">COUNTIF(D31:D53,"pass")</f>
+        <f t="shared" ref="D54:F54" si="9">COUNTIF(D31:D53,"pass")</f>
+        <v>20</v>
+      </c>
+      <c r="E54" s="10">
+        <f t="shared" si="9"/>
         <v>21</v>
       </c>
-      <c r="E54" s="10">
-        <f t="shared" si="7"/>
-        <v>21</v>
-      </c>
       <c r="F54" s="10">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G54" s="10">
+        <f t="shared" ref="G54" si="10">COUNTIF(G31:G53,"pass")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>143</v>
       </c>
@@ -3004,19 +3090,23 @@
         <v>1</v>
       </c>
       <c r="D55" s="5">
-        <f t="shared" ref="D55:F55" si="8">COUNTIF(D31:D53,"Ok")</f>
+        <f t="shared" ref="D55:F55" si="11">COUNTIF(D31:D53,"Ok")</f>
         <v>0</v>
       </c>
       <c r="E55" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F55" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G55" s="5">
+        <f t="shared" ref="G55" si="12">COUNTIF(G31:G53,"Ok")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>140</v>
       </c>
@@ -3029,19 +3119,23 @@
         <v>1</v>
       </c>
       <c r="D56" s="11">
-        <f t="shared" ref="D56:F56" si="9">COUNTIF(D31:D53,"workaround")</f>
+        <f t="shared" ref="D56:F56" si="13">COUNTIF(D31:D53,"workaround")</f>
         <v>1</v>
       </c>
       <c r="E56" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="F56" s="11">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G56" s="11">
+        <f t="shared" ref="G56" si="14">COUNTIF(G31:G53,"workaround")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>7</v>
       </c>
@@ -3054,19 +3148,23 @@
         <v>0</v>
       </c>
       <c r="D57" s="12">
-        <f t="shared" ref="D57:F57" si="10">COUNTIF(D31:D53,"Fail")</f>
+        <f t="shared" ref="D57:F57" si="15">COUNTIF(D31:D53,"Fail")</f>
         <v>1</v>
       </c>
       <c r="E57" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="F57" s="12">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="G57" s="12">
+        <f t="shared" ref="G57" si="16">COUNTIF(G31:G53,"Fail")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>145</v>
       </c>
@@ -3079,77 +3177,90 @@
         <v>0</v>
       </c>
       <c r="D58" s="2">
-        <f t="shared" ref="D58:F58" si="11">COUNT(D31:D53,"Untested")</f>
+        <f t="shared" ref="D58:F58" si="17">COUNT(D31:D53,"Untested")</f>
         <v>0</v>
       </c>
       <c r="E58" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="F58" s="2">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="G58" s="2">
+        <f t="shared" ref="G58" si="18">COUNT(G31:G53,"Untested")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>139</v>
       </c>
       <c r="B59" s="2">
         <f>B54+B57+B56+B58+B55</f>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C59" s="2">
         <f>C54+C57+C56+C58+C55</f>
         <v>23</v>
       </c>
       <c r="D59" s="2">
-        <f t="shared" ref="D59:F59" si="12">D54+D57+D56+D58+D55</f>
+        <f t="shared" ref="D59:F59" si="19">D54+D57+D56+D58+D55</f>
+        <v>22</v>
+      </c>
+      <c r="E59" s="2">
+        <f t="shared" si="19"/>
         <v>23</v>
       </c>
-      <c r="E59" s="2">
-        <f t="shared" si="12"/>
-        <v>23</v>
-      </c>
       <c r="F59" s="2">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="G59" s="2">
+        <f t="shared" ref="G59" si="20">G54+G57+G56+G58+G55</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B60" s="6">
         <f>(B54+B55)/B59</f>
-        <v>0.95652173913043481</v>
+        <v>0.95454545454545459</v>
       </c>
       <c r="C60" s="6">
         <f>(C54+C55)/C59</f>
         <v>0.95652173913043481</v>
       </c>
       <c r="D60" s="6">
-        <f t="shared" ref="D60:F60" si="13">(D54+D55)/D59</f>
+        <f t="shared" ref="D60:F60" si="21">(D54+D55)/D59</f>
+        <v>0.90909090909090906</v>
+      </c>
+      <c r="E60" s="6">
+        <f t="shared" si="21"/>
         <v>0.91304347826086951</v>
       </c>
-      <c r="E60" s="6">
-        <f t="shared" si="13"/>
-        <v>0.91304347826086951</v>
-      </c>
       <c r="F60" s="6" t="e">
-        <f t="shared" si="13"/>
+        <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G60" s="6" t="e">
+        <f t="shared" ref="G60" si="22">(G54+G55)/G59</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
-      <c r="B61" s="22"/>
-      <c r="C61" s="22"/>
-      <c r="D61" s="22"/>
-      <c r="E61" s="22"/>
-      <c r="F61" s="22"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B61" s="20"/>
+      <c r="C61" s="20"/>
+      <c r="D61" s="20"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="20"/>
+      <c r="G61" s="20"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>85</v>
       </c>
@@ -3158,8 +3269,9 @@
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G62" s="3"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>86</v>
       </c>
@@ -3176,8 +3288,9 @@
         <v>6</v>
       </c>
       <c r="F63" s="2"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G63" s="2"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>87</v>
       </c>
@@ -3194,8 +3307,9 @@
         <v>6</v>
       </c>
       <c r="F64" s="2"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G64" s="2"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>88</v>
       </c>
@@ -3212,8 +3326,9 @@
         <v>6</v>
       </c>
       <c r="F65" s="2"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G65" s="2"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>89</v>
       </c>
@@ -3230,8 +3345,9 @@
         <v>6</v>
       </c>
       <c r="F66" s="2"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G66" s="2"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>90</v>
       </c>
@@ -3248,8 +3364,9 @@
         <v>6</v>
       </c>
       <c r="F67" s="2"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G67" s="2"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>91</v>
       </c>
@@ -3266,8 +3383,9 @@
         <v>6</v>
       </c>
       <c r="F68" s="2"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G68" s="2"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>92</v>
       </c>
@@ -3284,26 +3402,28 @@
         <v>6</v>
       </c>
       <c r="F69" s="2"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G69" s="2"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="B70" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C70" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D70" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="E70" s="23" t="s">
+      <c r="B70" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C70" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E70" s="21" t="s">
         <v>6</v>
       </c>
       <c r="F70" s="15"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G70" s="15"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>6</v>
       </c>
@@ -3316,19 +3436,23 @@
         <v>8</v>
       </c>
       <c r="D71" s="10">
-        <f t="shared" ref="D71:F71" si="14">COUNTIF(D63:D70,"pass")</f>
+        <f t="shared" ref="D71:F71" si="23">COUNTIF(D63:D70,"pass")</f>
         <v>8</v>
       </c>
       <c r="E71" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>8</v>
       </c>
       <c r="F71" s="10">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="G71" s="10">
+        <f t="shared" ref="G71" si="24">COUNTIF(G63:G70,"pass")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>143</v>
       </c>
@@ -3341,44 +3465,52 @@
         <v>0</v>
       </c>
       <c r="D72" s="5">
-        <f t="shared" ref="D72:F72" si="15">COUNTIF(D63:D70,"Ok")</f>
+        <f t="shared" ref="D72:F72" si="25">COUNTIF(D63:D70,"Ok")</f>
         <v>0</v>
       </c>
       <c r="E72" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="F72" s="5">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="G72" s="5">
+        <f t="shared" ref="G72" si="26">COUNTIF(G63:G70,"Ok")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>140</v>
       </c>
       <c r="B73" s="11">
-        <f>COUNTIF(B94:B163,"workaround")</f>
+        <f t="shared" ref="B73:G73" si="27">COUNTIF(B94:B163,"workaround")</f>
         <v>1</v>
       </c>
       <c r="C73" s="11">
-        <f>COUNTIF(C94:C163,"workaround")</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="D73" s="11">
-        <f>COUNTIF(D94:D163,"workaround")</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="E73" s="11">
-        <f>COUNTIF(E94:E163,"workaround")</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="F73" s="11">
-        <f>COUNTIF(F94:F163,"workaround")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="G73" s="11">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>7</v>
       </c>
@@ -3391,19 +3523,23 @@
         <v>0</v>
       </c>
       <c r="D74" s="12">
-        <f t="shared" ref="D74:F74" si="16">COUNTIF(D63:D70,"Fail")</f>
+        <f t="shared" ref="D74:F74" si="28">COUNTIF(D63:D70,"Fail")</f>
         <v>0</v>
       </c>
       <c r="E74" s="12">
-        <f t="shared" si="16"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="F74" s="12">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="G74" s="12">
+        <f t="shared" ref="G74" si="29">COUNTIF(G63:G70,"Fail")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>145</v>
       </c>
@@ -3416,19 +3552,23 @@
         <v>0</v>
       </c>
       <c r="D75" s="2">
-        <f t="shared" ref="D75:F75" si="17">COUNT(D63:D70,"Untested")</f>
+        <f t="shared" ref="D75:F75" si="30">COUNT(D63:D70,"Untested")</f>
         <v>0</v>
       </c>
       <c r="E75" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="F75" s="2">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="G75" s="2">
+        <f t="shared" ref="G75" si="31">COUNT(G63:G70,"Untested")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>139</v>
       </c>
@@ -3441,19 +3581,23 @@
         <v>9</v>
       </c>
       <c r="D76" s="2">
-        <f t="shared" ref="D76:F76" si="18">D71+D74+D73+D75+D72</f>
+        <f t="shared" ref="D76:F76" si="32">D71+D74+D73+D75+D72</f>
         <v>9</v>
       </c>
       <c r="E76" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="32"/>
         <v>9</v>
       </c>
       <c r="F76" s="2">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="G76" s="2">
+        <f t="shared" ref="G76" si="33">G71+G74+G73+G75+G72</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="18" t="s">
         <v>8</v>
       </c>
@@ -3466,27 +3610,32 @@
         <v>0.88888888888888884</v>
       </c>
       <c r="D77" s="6">
-        <f t="shared" ref="D77:F77" si="19">(D71+D72)/D76</f>
+        <f t="shared" ref="D77:F77" si="34">(D71+D72)/D76</f>
         <v>0.88888888888888884</v>
       </c>
       <c r="E77" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="34"/>
         <v>0.88888888888888884</v>
       </c>
       <c r="F77" s="6" t="e">
-        <f t="shared" si="19"/>
+        <f t="shared" si="34"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G77" s="6" t="e">
+        <f t="shared" ref="G77" si="35">(G71+G72)/G76</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="13"/>
       <c r="B78" s="16"/>
       <c r="C78" s="16"/>
       <c r="D78" s="16"/>
       <c r="E78" s="16"/>
       <c r="F78" s="16"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G78" s="16"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="15" t="s">
         <v>64</v>
       </c>
@@ -3495,8 +3644,9 @@
       <c r="D79" s="15"/>
       <c r="E79" s="15"/>
       <c r="F79" s="15"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G79" s="15"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>65</v>
       </c>
@@ -3515,8 +3665,11 @@
       <c r="F80" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G80" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>67</v>
       </c>
@@ -3535,8 +3688,11 @@
       <c r="F81" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G81" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>68</v>
       </c>
@@ -3555,8 +3711,11 @@
       <c r="F82" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G82" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>69</v>
       </c>
@@ -3575,8 +3734,11 @@
       <c r="F83" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G83" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>70</v>
       </c>
@@ -3595,8 +3757,11 @@
       <c r="F84" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G84" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>71</v>
       </c>
@@ -3615,8 +3780,11 @@
       <c r="F85" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G85" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>72</v>
       </c>
@@ -3635,8 +3803,11 @@
       <c r="F86" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G86" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>73</v>
       </c>
@@ -3655,8 +3826,11 @@
       <c r="F87" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G87" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>74</v>
       </c>
@@ -3675,8 +3849,11 @@
       <c r="F88" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G88" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>75</v>
       </c>
@@ -3695,8 +3872,11 @@
       <c r="F89" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G89" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>76</v>
       </c>
@@ -3715,8 +3895,11 @@
       <c r="F90" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G90" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>77</v>
       </c>
@@ -3735,8 +3918,11 @@
       <c r="F91" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G91" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>78</v>
       </c>
@@ -3755,8 +3941,11 @@
       <c r="F92" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G92" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>79</v>
       </c>
@@ -3775,8 +3964,11 @@
       <c r="F93" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G93" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>80</v>
       </c>
@@ -3795,8 +3987,11 @@
       <c r="F94" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G94" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>81</v>
       </c>
@@ -3815,8 +4010,11 @@
       <c r="F95" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G95" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>82</v>
       </c>
@@ -3835,8 +4033,11 @@
       <c r="F96" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G96" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>83</v>
       </c>
@@ -3855,153 +4056,179 @@
       <c r="F97" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G97" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="B98" s="24" t="s">
+      <c r="B98" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="C98" s="24" t="s">
+      <c r="C98" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="D98" s="24" t="s">
+      <c r="D98" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="E98" s="24" t="s">
+      <c r="E98" s="22" t="s">
         <v>140</v>
       </c>
       <c r="F98" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G98" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B99" s="10">
-        <f>COUNTIF(B80:B98,"pass")</f>
+        <f t="shared" ref="B99:G99" si="36">COUNTIF(B80:B98,"pass")</f>
         <v>18</v>
       </c>
       <c r="C99" s="10">
-        <f>COUNTIF(C80:C98,"pass")</f>
+        <f t="shared" si="36"/>
         <v>18</v>
       </c>
       <c r="D99" s="10">
-        <f>COUNTIF(D80:D98,"pass")</f>
+        <f t="shared" si="36"/>
         <v>17</v>
       </c>
       <c r="E99" s="10">
-        <f>COUNTIF(E80:E98,"pass")</f>
+        <f t="shared" si="36"/>
         <v>17</v>
       </c>
       <c r="F99" s="10">
-        <f>COUNTIF(F80:F98,"pass")</f>
+        <f t="shared" si="36"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G99" s="10">
+        <f t="shared" si="36"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>143</v>
       </c>
       <c r="B100" s="5">
-        <f>COUNTIF(B80:B98,"Ok")</f>
+        <f t="shared" ref="B100:G100" si="37">COUNTIF(B80:B98,"Ok")</f>
         <v>0</v>
       </c>
       <c r="C100" s="5">
-        <f>COUNTIF(C80:C98,"Ok")</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="D100" s="5">
-        <f>COUNTIF(D80:D98,"Ok")</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="E100" s="5">
-        <f>COUNTIF(E80:E98,"Ok")</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="F100" s="5">
-        <f>COUNTIF(F80:F98,"Ok")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="G100" s="5">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>140</v>
       </c>
       <c r="B101" s="11">
-        <f>COUNTIF(B80:B98,"workaround")</f>
+        <f t="shared" ref="B101:G101" si="38">COUNTIF(B80:B98,"workaround")</f>
         <v>1</v>
       </c>
       <c r="C101" s="11">
-        <f>COUNTIF(C80:C98,"workaround")</f>
+        <f t="shared" si="38"/>
         <v>1</v>
       </c>
       <c r="D101" s="11">
-        <f>COUNTIF(D80:D98,"workaround")</f>
+        <f t="shared" si="38"/>
         <v>1</v>
       </c>
       <c r="E101" s="11">
-        <f>COUNTIF(E80:E98,"workaround")</f>
+        <f t="shared" si="38"/>
         <v>1</v>
       </c>
       <c r="F101" s="11">
-        <f>COUNTIF(F80:F98,"workaround")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="G101" s="11">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B102" s="12">
-        <f>COUNTIF(B80:B98,"Fail")</f>
+        <f t="shared" ref="B102:G102" si="39">COUNTIF(B80:B98,"Fail")</f>
         <v>0</v>
       </c>
       <c r="C102" s="12">
-        <f>COUNTIF(C80:C98,"Fail")</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="D102" s="12">
-        <f>COUNTIF(D80:D98,"Fail")</f>
+        <f t="shared" si="39"/>
         <v>1</v>
       </c>
       <c r="E102" s="12">
-        <f>COUNTIF(E80:E98,"Fail")</f>
+        <f t="shared" si="39"/>
         <v>1</v>
       </c>
       <c r="F102" s="12">
-        <f>COUNTIF(F80:F98,"Fail")</f>
+        <f t="shared" si="39"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G102" s="12">
+        <f t="shared" si="39"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>145</v>
       </c>
       <c r="B103" s="2">
-        <f>COUNT(B80:B98,"Untested")</f>
+        <f t="shared" ref="B103:G103" si="40">COUNT(B80:B98,"Untested")</f>
         <v>0</v>
       </c>
       <c r="C103" s="2">
-        <f>COUNT(C80:C98,"Untested")</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="D103" s="2">
-        <f>COUNT(D80:D98,"Untested")</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="E103" s="2">
-        <f>COUNT(E80:E98,"Untested")</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="F103" s="2">
-        <f>COUNT(F80:F98,"Untested")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="G103" s="2">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>139</v>
       </c>
@@ -4014,19 +4241,23 @@
         <v>19</v>
       </c>
       <c r="D104" s="2">
-        <f t="shared" ref="D104:F104" si="20">D99+D102+D101+D103+D100</f>
+        <f t="shared" ref="D104:F104" si="41">D99+D102+D101+D103+D100</f>
         <v>19</v>
       </c>
       <c r="E104" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="41"/>
         <v>19</v>
       </c>
       <c r="F104" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="41"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G104" s="2">
+        <f t="shared" ref="G104" si="42">G99+G102+G101+G103+G100</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="18" t="s">
         <v>8</v>
       </c>
@@ -4039,27 +4270,32 @@
         <v>0.94736842105263153</v>
       </c>
       <c r="D105" s="6">
-        <f t="shared" ref="D105:F105" si="21">(D99+D100)/D104</f>
+        <f t="shared" ref="D105:F105" si="43">(D99+D100)/D104</f>
         <v>0.89473684210526316</v>
       </c>
       <c r="E105" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="43"/>
         <v>0.89473684210526316</v>
       </c>
       <c r="F105" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="43"/>
         <v>0.73684210526315785</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G105" s="6">
+        <f t="shared" ref="G105" si="44">(G99+G100)/G104</f>
+        <v>0.94736842105263153</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="14"/>
       <c r="B106" s="14"/>
       <c r="C106" s="14"/>
       <c r="D106" s="14"/>
       <c r="E106" s="14"/>
       <c r="F106" s="14"/>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G106" s="14"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="15" t="s">
         <v>12</v>
       </c>
@@ -4068,8 +4304,9 @@
       <c r="D107" s="15"/>
       <c r="E107" s="15"/>
       <c r="F107" s="15"/>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G107" s="15"/>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>14</v>
       </c>
@@ -4088,8 +4325,11 @@
       <c r="F108" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G108" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>15</v>
       </c>
@@ -4108,8 +4348,11 @@
       <c r="F109" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G109" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>16</v>
       </c>
@@ -4128,8 +4371,11 @@
       <c r="F110" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G110" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>17</v>
       </c>
@@ -4148,8 +4394,11 @@
       <c r="F111" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G111" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>18</v>
       </c>
@@ -4168,8 +4417,11 @@
       <c r="F112" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G112" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>19</v>
       </c>
@@ -4188,8 +4440,11 @@
       <c r="F113" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G113" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>20</v>
       </c>
@@ -4208,8 +4463,11 @@
       <c r="F114" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G114" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>21</v>
       </c>
@@ -4228,8 +4486,11 @@
       <c r="F115" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G115" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>22</v>
       </c>
@@ -4248,8 +4509,11 @@
       <c r="F116" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G116" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>23</v>
       </c>
@@ -4268,8 +4532,11 @@
       <c r="F117" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G117" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>24</v>
       </c>
@@ -4288,8 +4555,11 @@
       <c r="F118" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G118" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>25</v>
       </c>
@@ -4308,8 +4578,11 @@
       <c r="F119" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G119" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>26</v>
       </c>
@@ -4328,8 +4601,11 @@
       <c r="F120" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G120" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>27</v>
       </c>
@@ -4348,8 +4624,11 @@
       <c r="F121" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G121" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>28</v>
       </c>
@@ -4368,8 +4647,11 @@
       <c r="F122" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G122" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>29</v>
       </c>
@@ -4388,8 +4670,11 @@
       <c r="F123" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G123" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>31</v>
       </c>
@@ -4408,8 +4693,11 @@
       <c r="F124" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G124" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>32</v>
       </c>
@@ -4428,8 +4716,11 @@
       <c r="F125" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G125" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>33</v>
       </c>
@@ -4448,8 +4739,11 @@
       <c r="F126" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G126" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>34</v>
       </c>
@@ -4468,8 +4762,11 @@
       <c r="F127" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G127" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>35</v>
       </c>
@@ -4488,8 +4785,11 @@
       <c r="F128" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G128" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>36</v>
       </c>
@@ -4508,8 +4808,11 @@
       <c r="F129" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G129" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>37</v>
       </c>
@@ -4528,8 +4831,11 @@
       <c r="F130" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G130" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>38</v>
       </c>
@@ -4548,8 +4854,11 @@
       <c r="F131" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G131" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>39</v>
       </c>
@@ -4568,8 +4877,11 @@
       <c r="F132" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G132" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>40</v>
       </c>
@@ -4588,8 +4900,11 @@
       <c r="F133" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G133" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>41</v>
       </c>
@@ -4608,8 +4923,11 @@
       <c r="F134" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G134" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>42</v>
       </c>
@@ -4628,8 +4946,11 @@
       <c r="F135" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G135" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>43</v>
       </c>
@@ -4648,8 +4969,11 @@
       <c r="F136" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G136" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>44</v>
       </c>
@@ -4668,8 +4992,11 @@
       <c r="F137" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G137" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>45</v>
       </c>
@@ -4688,8 +5015,11 @@
       <c r="F138" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G138" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>46</v>
       </c>
@@ -4708,8 +5038,11 @@
       <c r="F139" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G139" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>47</v>
       </c>
@@ -4728,8 +5061,11 @@
       <c r="F140" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G140" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>48</v>
       </c>
@@ -4748,8 +5084,11 @@
       <c r="F141" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G141" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>49</v>
       </c>
@@ -4768,8 +5107,11 @@
       <c r="F142" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G142" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>50</v>
       </c>
@@ -4788,8 +5130,11 @@
       <c r="F143" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G143" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>51</v>
       </c>
@@ -4808,8 +5153,11 @@
       <c r="F144" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G144" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>52</v>
       </c>
@@ -4828,8 +5176,11 @@
       <c r="F145" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G145" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>53</v>
       </c>
@@ -4848,8 +5199,11 @@
       <c r="F146" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G146" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>54</v>
       </c>
@@ -4868,8 +5222,11 @@
       <c r="F147" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G147" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>55</v>
       </c>
@@ -4888,8 +5245,11 @@
       <c r="F148" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G148" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>56</v>
       </c>
@@ -4908,8 +5268,11 @@
       <c r="F149" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G149" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>57</v>
       </c>
@@ -4928,8 +5291,11 @@
       <c r="F150" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G150" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>58</v>
       </c>
@@ -4948,8 +5314,11 @@
       <c r="F151" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G151" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>59</v>
       </c>
@@ -4968,8 +5337,11 @@
       <c r="F152" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G152" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>60</v>
       </c>
@@ -4988,8 +5360,11 @@
       <c r="F153" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G153" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>61</v>
       </c>
@@ -5008,8 +5383,11 @@
       <c r="F154" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G154" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>62</v>
       </c>
@@ -5028,153 +5406,179 @@
       <c r="F155" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G155" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="B156" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C156" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D156" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="E156" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="F156" s="23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B156" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C156" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D156" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E156" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F156" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G156" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B157" s="10">
-        <f>COUNTIF(B108:B156,"pass")</f>
+        <f t="shared" ref="B157:G157" si="45">COUNTIF(B108:B156,"pass")</f>
         <v>48</v>
       </c>
       <c r="C157" s="10">
-        <f>COUNTIF(C108:C156,"pass")</f>
+        <f t="shared" si="45"/>
         <v>48</v>
       </c>
       <c r="D157" s="10">
-        <f>COUNTIF(D108:D156,"pass")</f>
+        <f t="shared" si="45"/>
         <v>49</v>
       </c>
       <c r="E157" s="10">
-        <f>COUNTIF(E108:E156,"pass")</f>
+        <f t="shared" si="45"/>
         <v>49</v>
       </c>
       <c r="F157" s="10">
-        <f>COUNTIF(F108:F156,"pass")</f>
+        <f t="shared" si="45"/>
         <v>43</v>
       </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G157" s="10">
+        <f t="shared" si="45"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>143</v>
       </c>
       <c r="B158" s="5">
-        <f>COUNTIF(B108:B156,"Ok")</f>
+        <f t="shared" ref="B158:G158" si="46">COUNTIF(B108:B156,"Ok")</f>
         <v>1</v>
       </c>
       <c r="C158" s="5">
-        <f>COUNTIF(C108:C156,"Ok")</f>
+        <f t="shared" si="46"/>
         <v>1</v>
       </c>
       <c r="D158" s="5">
-        <f>COUNTIF(D108:D156,"Ok")</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="E158" s="5">
-        <f>COUNTIF(E108:E156,"Ok")</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="F158" s="5">
-        <f>COUNTIF(F108:F156,"Ok")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="G158" s="5">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>140</v>
       </c>
       <c r="B159" s="11">
-        <f>COUNTIF(B108:B156,"workaround")</f>
+        <f t="shared" ref="B159:G159" si="47">COUNTIF(B108:B156,"workaround")</f>
         <v>0</v>
       </c>
       <c r="C159" s="11">
-        <f>COUNTIF(C108:C156,"workaround")</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="D159" s="11">
-        <f>COUNTIF(D108:D156,"workaround")</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="E159" s="11">
-        <f>COUNTIF(E108:E156,"workaround")</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="F159" s="11">
-        <f>COUNTIF(F108:F156,"workaround")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="47"/>
+        <v>0</v>
+      </c>
+      <c r="G159" s="11">
+        <f t="shared" si="47"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B160" s="12">
-        <f>COUNTIF(B108:B156,"Fail")</f>
+        <f t="shared" ref="B160:G160" si="48">COUNTIF(B108:B156,"Fail")</f>
         <v>0</v>
       </c>
       <c r="C160" s="12">
-        <f>COUNTIF(C108:C156,"Fail")</f>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="D160" s="12">
-        <f>COUNTIF(D108:D156,"Fail")</f>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="E160" s="12">
-        <f>COUNTIF(E108:E156,"Fail")</f>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="F160" s="12">
-        <f>COUNTIF(F108:F156,"Fail")</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="48"/>
+        <v>6</v>
+      </c>
+      <c r="G160" s="12">
+        <f t="shared" si="48"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>145</v>
       </c>
       <c r="B161" s="2">
-        <f>COUNT(B108:B156,"Untested")</f>
+        <f t="shared" ref="B161:G161" si="49">COUNT(B108:B156,"Untested")</f>
         <v>0</v>
       </c>
       <c r="C161" s="2">
-        <f>COUNT(C108:C156,"Untested")</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="D161" s="2">
-        <f>COUNT(D108:D156,"Untested")</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="E161" s="2">
-        <f>COUNT(E108:E156,"Untested")</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="F161" s="2">
-        <f>COUNT(F108:F156,"Untested")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="49"/>
+        <v>0</v>
+      </c>
+      <c r="G161" s="2">
+        <f t="shared" si="49"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>139</v>
       </c>
@@ -5187,19 +5591,23 @@
         <v>49</v>
       </c>
       <c r="D162" s="2">
-        <f t="shared" ref="D162:F162" si="22">D157+D160+D159+D161+D158</f>
+        <f t="shared" ref="D162:F162" si="50">D157+D160+D159+D161+D158</f>
         <v>49</v>
       </c>
       <c r="E162" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="50"/>
         <v>49</v>
       </c>
       <c r="F162" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="50"/>
         <v>49</v>
       </c>
-    </row>
-    <row r="163" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G162" s="2">
+        <f t="shared" ref="G162" si="51">G157+G160+G159+G161+G158</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="18" t="s">
         <v>8</v>
       </c>
@@ -5212,27 +5620,32 @@
         <v>1</v>
       </c>
       <c r="D163" s="6">
-        <f t="shared" ref="D163:F163" si="23">(D157+D158)/D162</f>
+        <f t="shared" ref="D163:F163" si="52">(D157+D158)/D162</f>
         <v>1</v>
       </c>
       <c r="E163" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="52"/>
         <v>1</v>
       </c>
       <c r="F163" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="52"/>
         <v>0.87755102040816324</v>
       </c>
-    </row>
-    <row r="164" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G163" s="6">
+        <f t="shared" ref="G163" si="53">(G157+G158)/G162</f>
+        <v>0.93877551020408168</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="13"/>
       <c r="B164" s="16"/>
       <c r="C164" s="16"/>
       <c r="D164" s="13"/>
       <c r="E164" s="13"/>
       <c r="F164" s="13"/>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G164" s="13"/>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="19" t="s">
         <v>146</v>
       </c>
@@ -5241,8 +5654,9 @@
       <c r="D165" s="15"/>
       <c r="E165" s="15"/>
       <c r="F165" s="15"/>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G165" s="15"/>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>30</v>
       </c>
@@ -5259,9 +5673,10 @@
         <v>6</v>
       </c>
       <c r="F166" s="2"/>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A167" s="25" t="s">
+      <c r="G166" s="2"/>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A167" s="23" t="s">
         <v>156</v>
       </c>
       <c r="B167" s="4" t="s">
@@ -5273,8 +5688,9 @@
       <c r="D167" s="2"/>
       <c r="E167" s="2"/>
       <c r="F167" s="2"/>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G167" s="2"/>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>95</v>
       </c>
@@ -5287,8 +5703,9 @@
         <v>6</v>
       </c>
       <c r="F168" s="2"/>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G168" s="2"/>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>96</v>
       </c>
@@ -5301,8 +5718,9 @@
         <v>6</v>
       </c>
       <c r="F169" s="2"/>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G169" s="2"/>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>104</v>
       </c>
@@ -5315,8 +5733,9 @@
         <v>6</v>
       </c>
       <c r="F170" s="2"/>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G170" s="2"/>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>105</v>
       </c>
@@ -5329,8 +5748,9 @@
       <c r="D171" s="2"/>
       <c r="E171" s="2"/>
       <c r="F171" s="2"/>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G171" s="2"/>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>106</v>
       </c>
@@ -5343,8 +5763,9 @@
         <v>6</v>
       </c>
       <c r="F172" s="2"/>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G172" s="2"/>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>107</v>
       </c>
@@ -5361,8 +5782,9 @@
         <v>6</v>
       </c>
       <c r="F173" s="2"/>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G173" s="2"/>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>114</v>
       </c>
@@ -5375,8 +5797,9 @@
       <c r="D174" s="2"/>
       <c r="E174" s="2"/>
       <c r="F174" s="2"/>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G174" s="2"/>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>117</v>
       </c>
@@ -5389,8 +5812,9 @@
         <v>6</v>
       </c>
       <c r="F175" s="2"/>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G175" s="2"/>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>119</v>
       </c>
@@ -5403,8 +5827,9 @@
       <c r="D176" s="2"/>
       <c r="E176" s="2"/>
       <c r="F176" s="2"/>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G176" s="2"/>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>125</v>
       </c>
@@ -5417,22 +5842,24 @@
         <v>6</v>
       </c>
       <c r="F177" s="2"/>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G177" s="2"/>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="B178" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C178" s="23" t="s">
+      <c r="B178" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C178" s="21" t="s">
         <v>6</v>
       </c>
       <c r="D178" s="15"/>
       <c r="E178" s="15"/>
       <c r="F178" s="15"/>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G178" s="15"/>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>6</v>
       </c>
@@ -5445,19 +5872,23 @@
         <v>7</v>
       </c>
       <c r="D179" s="10">
-        <f t="shared" ref="D179:F179" si="24">COUNTIF(D166:D178,"pass")</f>
+        <f t="shared" ref="D179:F179" si="54">COUNTIF(D166:D178,"pass")</f>
         <v>8</v>
       </c>
       <c r="E179" s="10">
-        <f t="shared" si="24"/>
+        <f t="shared" si="54"/>
         <v>8</v>
       </c>
       <c r="F179" s="10">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="G179" s="10">
+        <f t="shared" ref="G179" si="55">COUNTIF(G166:G178,"pass")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>143</v>
       </c>
@@ -5470,19 +5901,23 @@
         <v>0</v>
       </c>
       <c r="D180" s="5">
-        <f t="shared" ref="D180:F180" si="25">COUNTIF(D166:D178,"Ok")</f>
+        <f t="shared" ref="D180:F180" si="56">COUNTIF(D166:D178,"Ok")</f>
         <v>0</v>
       </c>
       <c r="E180" s="5">
-        <f t="shared" si="25"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="F180" s="5">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="56"/>
+        <v>0</v>
+      </c>
+      <c r="G180" s="5">
+        <f t="shared" ref="G180" si="57">COUNTIF(G166:G178,"Ok")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>140</v>
       </c>
@@ -5495,19 +5930,23 @@
         <v>0</v>
       </c>
       <c r="D181" s="11">
-        <f t="shared" ref="D181:F181" si="26">COUNTIF(D166:D178,"workaround")</f>
+        <f t="shared" ref="D181:F181" si="58">COUNTIF(D166:D178,"workaround")</f>
         <v>0</v>
       </c>
       <c r="E181" s="11">
-        <f t="shared" si="26"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="F181" s="11">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="58"/>
+        <v>0</v>
+      </c>
+      <c r="G181" s="11">
+        <f t="shared" ref="G181" si="59">COUNTIF(G166:G178,"workaround")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>7</v>
       </c>
@@ -5520,19 +5959,23 @@
         <v>0</v>
       </c>
       <c r="D182" s="12">
-        <f t="shared" ref="D182:F182" si="27">COUNTIF(D166:D178,"Fail")</f>
+        <f t="shared" ref="D182:F182" si="60">COUNTIF(D166:D178,"Fail")</f>
         <v>0</v>
       </c>
       <c r="E182" s="12">
-        <f t="shared" si="27"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="F182" s="12">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="60"/>
+        <v>0</v>
+      </c>
+      <c r="G182" s="12">
+        <f t="shared" ref="G182" si="61">COUNTIF(G166:G178,"Fail")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>145</v>
       </c>
@@ -5545,19 +5988,23 @@
         <v>0</v>
       </c>
       <c r="D183" s="2">
-        <f t="shared" ref="D183:F183" si="28">COUNT(D166:D178,"Untested")</f>
+        <f t="shared" ref="D183:F183" si="62">COUNT(D166:D178,"Untested")</f>
         <v>0</v>
       </c>
       <c r="E183" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="F183" s="2">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="62"/>
+        <v>0</v>
+      </c>
+      <c r="G183" s="2">
+        <f t="shared" ref="G183" si="63">COUNT(G166:G178,"Untested")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>139</v>
       </c>
@@ -5570,19 +6017,23 @@
         <v>7</v>
       </c>
       <c r="D184" s="2">
-        <f t="shared" ref="D184:F184" si="29">D179+D182+D181+D183+D180</f>
+        <f t="shared" ref="D184:F184" si="64">D179+D182+D181+D183+D180</f>
         <v>8</v>
       </c>
       <c r="E184" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="64"/>
         <v>8</v>
       </c>
       <c r="F184" s="2">
-        <f t="shared" si="29"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="185" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="G184" s="2">
+        <f t="shared" ref="G184" si="65">G179+G182+G181+G183+G180</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="18" t="s">
         <v>8</v>
       </c>
@@ -5595,27 +6046,32 @@
         <v>1</v>
       </c>
       <c r="D185" s="6">
-        <f t="shared" ref="D185:F185" si="30">(D179+D180)/D184</f>
+        <f t="shared" ref="D185:F185" si="66">(D179+D180)/D184</f>
         <v>1</v>
       </c>
       <c r="E185" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="F185" s="6" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="66"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="186" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G185" s="6" t="e">
+        <f t="shared" ref="G185" si="67">(G179+G180)/G184</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="13"/>
       <c r="B186" s="13"/>
       <c r="C186" s="13"/>
       <c r="D186" s="13"/>
       <c r="E186" s="13"/>
       <c r="F186" s="13"/>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G186" s="13"/>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="15" t="s">
         <v>10</v>
       </c>
@@ -5624,8 +6080,9 @@
       <c r="D187" s="15"/>
       <c r="E187" s="15"/>
       <c r="F187" s="15"/>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G187" s="15"/>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>11</v>
       </c>
@@ -5640,8 +6097,11 @@
       <c r="F188" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G188" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>6</v>
       </c>
@@ -5654,19 +6114,23 @@
         <v>1</v>
       </c>
       <c r="D189" s="10">
-        <f t="shared" ref="D189:F189" si="31">COUNTIF(D188,"pass")</f>
+        <f t="shared" ref="D189:F189" si="68">COUNTIF(D188,"pass")</f>
         <v>0</v>
       </c>
       <c r="E189" s="10">
-        <f t="shared" si="31"/>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="F189" s="10">
-        <f t="shared" si="31"/>
+        <f t="shared" si="68"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G189" s="10">
+        <f t="shared" ref="G189" si="69">COUNTIF(G188,"pass")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>143</v>
       </c>
@@ -5679,19 +6143,23 @@
         <v>0</v>
       </c>
       <c r="D190" s="5">
-        <f t="shared" ref="D190:F190" si="32">COUNTIF(D188,"Ok")</f>
+        <f t="shared" ref="D190:F190" si="70">COUNTIF(D188,"Ok")</f>
         <v>0</v>
       </c>
       <c r="E190" s="5">
-        <f t="shared" si="32"/>
+        <f t="shared" si="70"/>
         <v>0</v>
       </c>
       <c r="F190" s="5">
-        <f t="shared" si="32"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="70"/>
+        <v>0</v>
+      </c>
+      <c r="G190" s="5">
+        <f t="shared" ref="G190" si="71">COUNTIF(G188,"Ok")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>140</v>
       </c>
@@ -5704,19 +6172,23 @@
         <v>0</v>
       </c>
       <c r="D191" s="11">
-        <f t="shared" ref="D191:F191" si="33">COUNTIF(D188,"workaround")</f>
+        <f t="shared" ref="D191:F191" si="72">COUNTIF(D188,"workaround")</f>
         <v>0</v>
       </c>
       <c r="E191" s="11">
-        <f t="shared" si="33"/>
+        <f t="shared" si="72"/>
         <v>0</v>
       </c>
       <c r="F191" s="11">
-        <f t="shared" si="33"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="72"/>
+        <v>0</v>
+      </c>
+      <c r="G191" s="11">
+        <f t="shared" ref="G191" si="73">COUNTIF(G188,"workaround")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>7</v>
       </c>
@@ -5729,19 +6201,23 @@
         <v>0</v>
       </c>
       <c r="D192" s="12">
-        <f t="shared" ref="D192:F192" si="34">COUNTIF(D188,"Fail")</f>
+        <f t="shared" ref="D192:F192" si="74">COUNTIF(D188,"Fail")</f>
         <v>0</v>
       </c>
       <c r="E192" s="12">
-        <f t="shared" si="34"/>
+        <f t="shared" si="74"/>
         <v>0</v>
       </c>
       <c r="F192" s="12">
-        <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="74"/>
+        <v>0</v>
+      </c>
+      <c r="G192" s="12">
+        <f t="shared" ref="G192" si="75">COUNTIF(G188,"Fail")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>145</v>
       </c>
@@ -5754,19 +6230,23 @@
         <v>0</v>
       </c>
       <c r="D193" s="2">
-        <f t="shared" ref="D193:F193" si="35">COUNT(D188,"Untested")</f>
+        <f t="shared" ref="D193:F193" si="76">COUNT(D188,"Untested")</f>
         <v>0</v>
       </c>
       <c r="E193" s="2">
-        <f t="shared" si="35"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="F193" s="2">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="76"/>
+        <v>0</v>
+      </c>
+      <c r="G193" s="2">
+        <f t="shared" ref="G193" si="77">COUNT(G188,"Untested")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>139</v>
       </c>
@@ -5779,19 +6259,23 @@
         <v>1</v>
       </c>
       <c r="D194" s="2">
-        <f t="shared" ref="D194:F194" si="36">D189+D192+D191+D193+D190</f>
+        <f t="shared" ref="D194:F194" si="78">D189+D192+D191+D193+D190</f>
         <v>0</v>
       </c>
       <c r="E194" s="2">
-        <f t="shared" si="36"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="F194" s="2">
-        <f t="shared" si="36"/>
+        <f t="shared" si="78"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="195" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G194" s="2">
+        <f t="shared" ref="G194" si="79">G189+G192+G191+G193+G190</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A195" s="18" t="s">
         <v>8</v>
       </c>
@@ -5804,22 +6288,27 @@
         <v>1</v>
       </c>
       <c r="D195" s="6" t="e">
-        <f t="shared" ref="D195:F195" si="37">(D189+D190)/D194</f>
+        <f t="shared" ref="D195:F195" si="80">(D189+D190)/D194</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E195" s="6" t="e">
-        <f t="shared" si="37"/>
+        <f t="shared" si="80"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F195" s="6">
-        <f t="shared" si="37"/>
+        <f t="shared" si="80"/>
         <v>1</v>
       </c>
+      <c r="G195" s="6">
+        <f t="shared" ref="G195" si="81">(G189+G190)/G194</f>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -5847,14 +6336,14 @@
       <c r="A1" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="E1" s="21"/>
+      <c r="E1" s="26"/>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -6092,10 +6581,10 @@
       <c r="A20" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="23" t="s">
+      <c r="B20" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="21" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="15"/>
@@ -6250,10 +6739,10 @@
     </row>
     <row r="28" spans="1:5" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
@@ -6642,16 +7131,16 @@
       <c r="A52" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="B52" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C52" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D52" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="E52" s="23" t="s">
+      <c r="B52" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" s="21" t="s">
         <v>6</v>
       </c>
     </row>
@@ -6804,10 +7293,10 @@
     </row>
     <row r="60" spans="1:5" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
-      <c r="B60" s="22"/>
-      <c r="C60" s="22"/>
-      <c r="D60" s="22"/>
-      <c r="E60" s="22"/>
+      <c r="B60" s="20"/>
+      <c r="C60" s="20"/>
+      <c r="D60" s="20"/>
+      <c r="E60" s="20"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
@@ -6941,16 +7430,16 @@
       <c r="A69" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="B69" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C69" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D69" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="E69" s="23" t="s">
+      <c r="B69" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C69" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E69" s="21" t="s">
         <v>6</v>
       </c>
     </row>
@@ -7461,16 +7950,16 @@
       <c r="A99" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="B99" s="24" t="s">
+      <c r="B99" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="C99" s="24" t="s">
+      <c r="C99" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="D99" s="24" t="s">
+      <c r="D99" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="E99" s="24" t="s">
+      <c r="E99" s="22" t="s">
         <v>140</v>
       </c>
     </row>
@@ -8474,16 +8963,16 @@
       <c r="A158" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="B158" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C158" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D158" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="E158" s="23" t="s">
+      <c r="B158" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C158" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D158" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E158" s="21" t="s">
         <v>6</v>
       </c>
     </row>
@@ -8805,10 +9294,10 @@
       <c r="A179" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="B179" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C179" s="23" t="s">
+      <c r="B179" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C179" s="21" t="s">
         <v>6</v>
       </c>
       <c r="D179" s="15"/>

</xml_diff>

<commit_message>
Written OpenGL status post
</commit_message>
<xml_diff>
--- a/doc/OpenGL status.xlsx
+++ b/doc/OpenGL status.xlsx
@@ -13,7 +13,6 @@
     <sheet name="2012-11" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -3604,6 +3603,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3623,12 +3628,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3993,11 +3992,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="77510144"/>
-        <c:axId val="77511680"/>
+        <c:axId val="153696128"/>
+        <c:axId val="153697664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="77510144"/>
+        <c:axId val="153696128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4006,7 +4005,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77511680"/>
+        <c:crossAx val="153697664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4014,7 +4013,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77511680"/>
+        <c:axId val="153697664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4026,7 +4025,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77510144"/>
+        <c:crossAx val="153696128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4534,11 +4533,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="78265344"/>
-        <c:axId val="78267136"/>
+        <c:axId val="154365312"/>
+        <c:axId val="154371200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="78265344"/>
+        <c:axId val="154365312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4547,7 +4546,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78267136"/>
+        <c:crossAx val="154371200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4555,7 +4554,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78267136"/>
+        <c:axId val="154371200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4567,7 +4566,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78265344"/>
+        <c:crossAx val="154365312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5038,11 +5037,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="78492416"/>
-        <c:axId val="78493952"/>
+        <c:axId val="154969216"/>
+        <c:axId val="154970752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="78492416"/>
+        <c:axId val="154969216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5051,7 +5050,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78493952"/>
+        <c:crossAx val="154970752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5059,7 +5058,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78493952"/>
+        <c:axId val="154970752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -5071,7 +5070,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78492416"/>
+        <c:crossAx val="154969216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5488,8 +5487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5503,22 +5502,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="41" t="s">
         <v>197</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="40" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
@@ -5554,7 +5553,7 @@
       <c r="C5" s="17">
         <v>41324</v>
       </c>
-      <c r="D5" s="46">
+      <c r="D5" s="39">
         <v>41296</v>
       </c>
       <c r="E5" s="17">
@@ -8104,7 +8103,7 @@
       <c r="D160" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E160" s="45" t="s">
+      <c r="E160" s="38" t="s">
         <v>140</v>
       </c>
     </row>
@@ -8172,7 +8171,7 @@
       <c r="D164" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E164" s="45" t="s">
+      <c r="E164" s="38" t="s">
         <v>140</v>
       </c>
     </row>
@@ -8274,7 +8273,7 @@
       <c r="D170" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E170" s="45" t="s">
+      <c r="E170" s="38" t="s">
         <v>140</v>
       </c>
     </row>
@@ -8291,7 +8290,7 @@
       <c r="D171" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E171" s="45" t="s">
+      <c r="E171" s="38" t="s">
         <v>140</v>
       </c>
     </row>
@@ -8342,7 +8341,7 @@
       <c r="D174" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E174" s="45" t="s">
+      <c r="E174" s="38" t="s">
         <v>140</v>
       </c>
     </row>
@@ -8359,7 +8358,7 @@
       <c r="D175" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E175" s="45" t="s">
+      <c r="E175" s="38" t="s">
         <v>140</v>
       </c>
     </row>
@@ -8563,7 +8562,7 @@
       <c r="D187" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E187" s="45" t="s">
+      <c r="E187" s="38" t="s">
         <v>140</v>
       </c>
     </row>
@@ -8580,7 +8579,7 @@
       <c r="D188" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E188" s="45" t="s">
+      <c r="E188" s="38" t="s">
         <v>140</v>
       </c>
     </row>
@@ -8784,7 +8783,7 @@
       <c r="D200" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E200" s="45" t="s">
+      <c r="E200" s="38" t="s">
         <v>140</v>
       </c>
     </row>
@@ -9503,26 +9502,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="40" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
@@ -9537,18 +9536,18 @@
       <c r="A4" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="42" t="s">
+      <c r="C4" s="43"/>
+      <c r="D4" s="44" t="s">
         <v>151</v>
       </c>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42" t="s">
+      <c r="E4" s="44"/>
+      <c r="F4" s="44" t="s">
         <v>150</v>
       </c>
-      <c r="G4" s="42"/>
+      <c r="G4" s="44"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -14850,26 +14849,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="41" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="40" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
@@ -14884,18 +14883,18 @@
       <c r="A4" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="42" t="s">
+      <c r="C4" s="43"/>
+      <c r="D4" s="44" t="s">
         <v>151</v>
       </c>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42" t="s">
+      <c r="E4" s="44"/>
+      <c r="F4" s="44" t="s">
         <v>150</v>
       </c>
-      <c r="G4" s="42"/>
+      <c r="G4" s="44"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -19556,14 +19555,14 @@
       <c r="A1" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="44" t="s">
+      <c r="C1" s="45"/>
+      <c r="D1" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="E1" s="44"/>
+      <c r="E1" s="46"/>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">

</xml_diff>

<commit_message>
Added September OpenGL status
</commit_message>
<xml_diff>
--- a/doc/OpenGL status.xlsx
+++ b/doc/OpenGL status.xlsx
@@ -25,6 +25,20 @@
     <author>Groove</author>
   </authors>
   <commentList>
+    <comment ref="B39" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Doesn't support const expression arithmetic: C1154: non constant expression in layout value</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B52" authorId="0">
       <text>
         <r>
@@ -5682,6 +5696,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5703,7 +5718,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma 2" xfId="3"/>
@@ -5811,7 +5825,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.35714285714285715</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.9285714285714286</c:v>
@@ -6090,11 +6104,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="109782016"/>
-        <c:axId val="108505344"/>
+        <c:axId val="100925440"/>
+        <c:axId val="95673088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="109782016"/>
+        <c:axId val="100925440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6103,7 +6117,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108505344"/>
+        <c:crossAx val="95673088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6111,7 +6125,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108505344"/>
+        <c:axId val="95673088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -6123,7 +6137,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109782016"/>
+        <c:crossAx val="100925440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6479,11 +6493,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="4076032"/>
-        <c:axId val="95673664"/>
+        <c:axId val="100493312"/>
+        <c:axId val="108504192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="4076032"/>
+        <c:axId val="100493312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6492,7 +6506,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95673664"/>
+        <c:crossAx val="108504192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6500,7 +6514,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95673664"/>
+        <c:axId val="108504192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -6512,7 +6526,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="4076032"/>
+        <c:crossAx val="100493312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6867,11 +6881,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="133890048"/>
-        <c:axId val="105631104"/>
+        <c:axId val="104706048"/>
+        <c:axId val="108508224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="133890048"/>
+        <c:axId val="104706048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6880,7 +6894,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105631104"/>
+        <c:crossAx val="108508224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6888,7 +6902,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105631104"/>
+        <c:axId val="108508224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -6900,7 +6914,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133890048"/>
+        <c:crossAx val="104706048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7255,11 +7269,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="100491264"/>
-        <c:axId val="105633984"/>
+        <c:axId val="101021184"/>
+        <c:axId val="109209856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="100491264"/>
+        <c:axId val="101021184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7268,7 +7282,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105633984"/>
+        <c:crossAx val="109209856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7276,7 +7290,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105633984"/>
+        <c:axId val="109209856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -7288,7 +7302,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100491264"/>
+        <c:crossAx val="101021184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7795,11 +7809,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="100494848"/>
-        <c:axId val="114820224"/>
+        <c:axId val="120729088"/>
+        <c:axId val="109213312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="100494848"/>
+        <c:axId val="120729088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7808,7 +7822,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114820224"/>
+        <c:crossAx val="109213312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7816,7 +7830,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114820224"/>
+        <c:axId val="109213312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -7828,7 +7842,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100494848"/>
+        <c:crossAx val="120729088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8299,11 +8313,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="101019648"/>
-        <c:axId val="114821952"/>
+        <c:axId val="130683904"/>
+        <c:axId val="104284160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="101019648"/>
+        <c:axId val="130683904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8312,7 +8326,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114821952"/>
+        <c:crossAx val="104284160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8320,7 +8334,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114821952"/>
+        <c:axId val="104284160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -8332,14 +8346,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101019648"/>
+        <c:crossAx val="130683904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8861,8 +8874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E259"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8876,22 +8889,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>332</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
@@ -8996,19 +9009,19 @@
       <c r="A10" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="B10" s="56">
-        <f>IF(B$47=0, 0,(B$42+B$43)/B$70)</f>
-        <v>0.35714285714285715</v>
-      </c>
-      <c r="C10" s="56">
-        <f t="shared" ref="C10:E10" si="0">IF(C$47=0, 0,(C$42+C$43)/C$70)</f>
-        <v>0</v>
-      </c>
-      <c r="D10" s="56">
+      <c r="B10" s="49">
+        <f>IF(B$47=0, 0,(B$42+B$43)/B$47)</f>
+        <v>0.8</v>
+      </c>
+      <c r="C10" s="49">
+        <f t="shared" ref="C10:E10" si="0">IF(C$47=0, 0,(C$42+C$43)/C$47)</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="49">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E10" s="56">
+      <c r="E10" s="49">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -9325,8 +9338,8 @@
       <c r="A39" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B39" s="4" t="s">
-        <v>6</v>
+      <c r="B39" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="C39" s="48" t="s">
         <v>177</v>
@@ -9378,7 +9391,7 @@
       </c>
       <c r="B42" s="10">
         <f>COUNTIF(B37:B41,"pass")</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C42" s="10">
         <f>COUNTIF(C37:C41,"pass")</f>
@@ -9441,7 +9454,7 @@
       </c>
       <c r="B45" s="12">
         <f>COUNTIF(B37:B41,"Fail")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C45" s="12">
         <f>COUNTIF(C37:C41,"Fail")</f>
@@ -9503,11 +9516,11 @@
         <v>8</v>
       </c>
       <c r="B48" s="6">
-        <f>IF(B$47=0, 0,(B$42+B$43)/B$70)</f>
-        <v>0.35714285714285715</v>
+        <f>IF(B$47=0, 0,(B$42+B$43)/B$47)</f>
+        <v>0.8</v>
       </c>
       <c r="C48" s="6">
-        <f t="shared" ref="C48:E48" si="1">IF(C$47=0, 0,(C$42+C$43)/C$70)</f>
+        <f t="shared" ref="C48:E48" si="1">IF(C$47=0, 0,(C$42+C$43)/C$47)</f>
         <v>0</v>
       </c>
       <c r="D48" s="6">
@@ -13152,22 +13165,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>330</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
@@ -17151,22 +17164,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>318</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
@@ -21150,22 +21163,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>197</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
@@ -25150,26 +25163,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
@@ -25184,18 +25197,18 @@
       <c r="A4" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="52"/>
-      <c r="D4" s="53" t="s">
+      <c r="C4" s="53"/>
+      <c r="D4" s="54" t="s">
         <v>151</v>
       </c>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53" t="s">
+      <c r="E4" s="54"/>
+      <c r="F4" s="54" t="s">
         <v>150</v>
       </c>
-      <c r="G4" s="53"/>
+      <c r="G4" s="54"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -30497,26 +30510,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
@@ -30531,18 +30544,18 @@
       <c r="A4" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="52"/>
-      <c r="D4" s="53" t="s">
+      <c r="C4" s="53"/>
+      <c r="D4" s="54" t="s">
         <v>151</v>
       </c>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53" t="s">
+      <c r="E4" s="54"/>
+      <c r="F4" s="54" t="s">
         <v>150</v>
       </c>
-      <c r="G4" s="53"/>
+      <c r="G4" s="54"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -35203,14 +35216,14 @@
       <c r="A1" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="55" t="s">
+      <c r="C1" s="55"/>
+      <c r="D1" s="56" t="s">
         <v>151</v>
       </c>
-      <c r="E1" s="55"/>
+      <c r="E1" s="56"/>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">

</xml_diff>

<commit_message>
Added picture 45 and 44
</commit_message>
<xml_diff>
--- a/doc/OpenGL status.xlsx
+++ b/doc/OpenGL status.xlsx
@@ -354,6 +354,21 @@
         </r>
       </text>
     </comment>
+    <comment ref="C128" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Require glDrawBuffer(GL_NONE) before glCheckFramebuffer otherwise the implementation generates an OpenGL error
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E128" authorId="0">
       <text>
         <r>
@@ -650,6 +665,21 @@
             <charset val="1"/>
           </rPr>
           <t>Render a black screen</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C191" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Require glDrawBuffer(GL_NONE) before glCheckFramebuffer otherwise the implementation generates an OpenGL error
+</t>
         </r>
       </text>
     </comment>
@@ -6684,13 +6714,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.95238095238095233</c:v>
+                  <c:v>0.90476190476190477</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.91111111111111109</c:v>
+                  <c:v>0.88888888888888884</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6869,11 +6899,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="158217728"/>
-        <c:axId val="111907904"/>
+        <c:axId val="146048512"/>
+        <c:axId val="146292736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="158217728"/>
+        <c:axId val="146048512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6882,7 +6912,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111907904"/>
+        <c:crossAx val="146292736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6890,7 +6920,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111907904"/>
+        <c:axId val="146292736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -6902,7 +6932,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="158217728"/>
+        <c:crossAx val="146048512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7282,11 +7312,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="61894656"/>
-        <c:axId val="114634112"/>
+        <c:axId val="84035072"/>
+        <c:axId val="146295040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="61894656"/>
+        <c:axId val="84035072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7295,7 +7325,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114634112"/>
+        <c:crossAx val="146295040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7303,7 +7333,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114634112"/>
+        <c:axId val="146295040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -7315,7 +7345,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61894656"/>
+        <c:crossAx val="84035072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7670,11 +7700,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="61896704"/>
-        <c:axId val="151330816"/>
+        <c:axId val="146974720"/>
+        <c:axId val="146297920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="61896704"/>
+        <c:axId val="146974720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7683,7 +7713,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151330816"/>
+        <c:crossAx val="146297920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7691,7 +7721,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="151330816"/>
+        <c:axId val="146297920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -7703,7 +7733,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61896704"/>
+        <c:crossAx val="146974720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8058,11 +8088,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="61895168"/>
-        <c:axId val="151332544"/>
+        <c:axId val="146972672"/>
+        <c:axId val="147177472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="61895168"/>
+        <c:axId val="146972672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8071,7 +8101,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151332544"/>
+        <c:crossAx val="147177472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8079,7 +8109,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="151332544"/>
+        <c:axId val="147177472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -8091,7 +8121,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61895168"/>
+        <c:crossAx val="146972672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8446,11 +8476,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="144461312"/>
-        <c:axId val="62122240"/>
+        <c:axId val="148200960"/>
+        <c:axId val="147180928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="144461312"/>
+        <c:axId val="148200960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8459,7 +8489,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62122240"/>
+        <c:crossAx val="147180928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8467,7 +8497,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62122240"/>
+        <c:axId val="147180928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -8479,7 +8509,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144461312"/>
+        <c:crossAx val="148200960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8986,11 +9016,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="145143296"/>
-        <c:axId val="62124544"/>
+        <c:axId val="148522496"/>
+        <c:axId val="147182656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="145143296"/>
+        <c:axId val="148522496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8999,7 +9029,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62124544"/>
+        <c:crossAx val="147182656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9007,7 +9037,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62124544"/>
+        <c:axId val="147182656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -9019,7 +9049,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145143296"/>
+        <c:crossAx val="148522496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9490,11 +9520,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="145144832"/>
-        <c:axId val="62126848"/>
+        <c:axId val="148524032"/>
+        <c:axId val="147184960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="145144832"/>
+        <c:axId val="148524032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9503,7 +9533,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62126848"/>
+        <c:crossAx val="147184960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9511,7 +9541,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62126848"/>
+        <c:axId val="147184960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -9523,7 +9553,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145144832"/>
+        <c:crossAx val="148524032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10088,8 +10118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E260"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C154" sqref="C154"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="I122" sqref="I122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10313,7 +10343,7 @@
       </c>
       <c r="C14" s="20">
         <f>IF(C$148=0, 0, (C$143+C$144)/C$148)</f>
-        <v>0.95238095238095233</v>
+        <v>0.90476190476190477</v>
       </c>
       <c r="D14" s="20">
         <f>IF(D$148=0, 0, (D$143+D$144)/D$148)</f>
@@ -10355,7 +10385,7 @@
       </c>
       <c r="C16" s="25">
         <f>IF(C$223=0, 0, (C$218+C$219)/C$223)</f>
-        <v>0.91111111111111109</v>
+        <v>0.88888888888888884</v>
       </c>
       <c r="D16" s="25">
         <f>IF(D$223=0, 0, (D$218+D$219)/D$223)</f>
@@ -12138,8 +12168,8 @@
       <c r="B128" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C128" s="4" t="s">
-        <v>6</v>
+      <c r="C128" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="D128" s="4" t="s">
         <v>6</v>
@@ -12396,7 +12426,7 @@
       </c>
       <c r="C143" s="10">
         <f>COUNTIF(C122:C142,"pass")</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D143" s="10">
         <f>COUNTIF(D122:D142,"pass")</f>
@@ -12459,7 +12489,7 @@
       </c>
       <c r="C146" s="12">
         <f>COUNTIF(C122:C142,"Fail")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D146" s="12">
         <f>COUNTIF(D122:D142,"Fail")</f>
@@ -12522,7 +12552,7 @@
       </c>
       <c r="C149" s="6">
         <f>IF(C$148=0, 0, (C$143+C$144)/C$148)</f>
-        <v>0.95238095238095233</v>
+        <v>0.90476190476190477</v>
       </c>
       <c r="D149" s="6">
         <f>IF(D$148=0, 0, (D$143+D$144)/D$148)</f>
@@ -13245,8 +13275,8 @@
       <c r="B191" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C191" s="4" t="s">
-        <v>6</v>
+      <c r="C191" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="D191" s="4" t="s">
         <v>6</v>
@@ -13707,7 +13737,7 @@
       </c>
       <c r="C218" s="10">
         <f>COUNTIF(C$173:C$217,"pass")</f>
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D218" s="10">
         <f>COUNTIF(D$173:D$217,"pass")</f>
@@ -13770,7 +13800,7 @@
       </c>
       <c r="C221" s="12">
         <f>COUNTIF(C173:C217,"Fail")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D221" s="12">
         <f>COUNTIF(D173:D217,"Fail")</f>
@@ -13833,7 +13863,7 @@
       </c>
       <c r="C224" s="6">
         <f>IF(C$223=0, 0, (C$218+C$219)/C$223)</f>
-        <v>0.91111111111111109</v>
+        <v>0.88888888888888884</v>
       </c>
       <c r="D224" s="6">
         <f>IF(D$223=0, 0, (D$218+D$219)/D$223)</f>

</xml_diff>

<commit_message>
Added february OpenGL status draft
</commit_message>
<xml_diff>
--- a/doc/OpenGL status.xlsx
+++ b/doc/OpenGL status.xlsx
@@ -127,6 +127,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="C59" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>OpenGL drivers crashes</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D59" authorId="0">
       <text>
         <r>
@@ -179,8 +193,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Driver hang
-</t>
+          <t>OpenGL drivers hang</t>
         </r>
       </text>
     </comment>
@@ -236,7 +249,22 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Quality is really bad
+          <t xml:space="preserve">Quality is unacceptable
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D92" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Produce rendering artifacts
 </t>
         </r>
       </text>
@@ -266,8 +294,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Offset and stride kind of problem when fetching the texture
-</t>
+          <t>Compressed tile copy is not correct</t>
         </r>
       </text>
     </comment>
@@ -555,20 +582,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="C175" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Fixed in this drivers</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="E186" authorId="0">
       <text>
         <r>
@@ -635,7 +648,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>The driver doesn't output vec4(0, 0, 0, 1) when the resolved interger color buffer is incomplete</t>
         </r>
@@ -670,6 +683,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="E195" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Generate an invalid operation error when on shadow rendering draw call.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E196" authorId="0">
       <text>
         <r>
@@ -694,8 +721,39 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">
-</t>
+          <t>"lowp int Count = lowp int(COUNT);" should generate an error.
+The valid form is:
+"lowp int Count = int(COUNT);"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D198" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>"lowp int Count = lowp int(COUNT);" should generate an error.
+The valid form is:
+"lowp int Count = int(COUNT);"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B201" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>NVIDIA compiler aspects a structure for the vertex input interface, This is not allowed, it would be nice to have an extension for it.</t>
         </r>
       </text>
     </comment>
@@ -707,13 +765,16 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t>Pop free clipping</t>
+          <t xml:space="preserve">glClearBufferfv is always performed, even is the condition fails.
+OpenGL 4.3 - 10.10 Conditional Rendering:
+Doesn't generate an GLSL compiler error when geometry shader input layout qualifier is missing
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="E207" authorId="0">
+    <comment ref="C205" authorId="0">
       <text>
         <r>
           <rPr>
@@ -723,7 +784,24 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Deleting shader object after being attached lead to invalid operations error generated when the program pop the stack</t>
+          <t xml:space="preserve">glClearBufferfv is always performed, even is the condition fails.
+OpenGL 4.3 - 10.10 Conditional Rendering:
+Doesn't generate an GLSL compiler error when geometry shader input layout qualifier is missing
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B206" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Pop free clipping</t>
         </r>
       </text>
     </comment>
@@ -741,7 +819,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C209" authorId="0">
+    <comment ref="C210" authorId="0">
       <text>
         <r>
           <rPr>
@@ -759,7 +837,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B220" authorId="0">
+    <comment ref="B221" authorId="0">
       <text>
         <r>
           <rPr>
@@ -773,7 +851,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E221" authorId="0">
+    <comment ref="E222" authorId="0">
       <text>
         <r>
           <rPr>
@@ -788,7 +866,21 @@
         </r>
       </text>
     </comment>
-    <comment ref="C237" authorId="0">
+    <comment ref="D244" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Affect the clearing of the framebuffer with an unexpected manner.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C251" authorId="0">
       <text>
         <r>
           <rPr>
@@ -802,7 +894,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D237" authorId="0">
+    <comment ref="D251" authorId="0">
       <text>
         <r>
           <rPr>
@@ -816,7 +908,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E237" authorId="0">
+    <comment ref="E251" authorId="0">
       <text>
         <r>
           <rPr>
@@ -827,20 +919,6 @@
             <family val="2"/>
           </rPr>
           <t>GL_NV_gpu_shader5 not supported</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D243" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Affect the clearing of the framebuffer with an unexpected manner.</t>
         </r>
       </text>
     </comment>
@@ -5938,7 +6016,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7155" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7181" uniqueCount="367">
   <si>
     <t>gl-430-texture-view</t>
   </si>
@@ -7017,7 +7095,28 @@
     <t>program-uniform</t>
   </si>
   <si>
-    <t>glsl-precision-cast</t>
+    <t>glsl-cast-fail</t>
+  </si>
+  <si>
+    <t>glsl-input-struct</t>
+  </si>
+  <si>
+    <t>320-texture-compressed-ext</t>
+  </si>
+  <si>
+    <t>330-sampler-anisotropic-ext</t>
+  </si>
+  <si>
+    <t>430-perf-monitor-amd</t>
+  </si>
+  <si>
+    <t>02/18/2013</t>
+  </si>
+  <si>
+    <t>334.89</t>
+  </si>
+  <si>
+    <t>NVIDIA 334.89</t>
   </si>
 </sst>
 </file>
@@ -7224,7 +7323,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -7353,6 +7452,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7373,6 +7474,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -7432,7 +7536,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>NVIDIA 331.10 beta</c:v>
+                  <c:v>NVIDIA 334.89</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7499,7 +7603,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.98</c:v>
+                  <c:v>0.94339622641509435</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7566,7 +7670,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.875</c:v>
@@ -7578,10 +7682,10 @@
                   <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0.91666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.9</c:v>
+                  <c:v>0.86792452830188682</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7651,10 +7755,10 @@
                   <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.875</c:v>
+                  <c:v>0.83333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0.8571428571428571</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.95</c:v>
@@ -7663,7 +7767,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.98</c:v>
+                  <c:v>0.96226415094339623</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7745,7 +7849,7 @@
                   <c:v>0.91666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.9</c:v>
+                  <c:v>0.90196078431372551</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7760,11 +7864,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="66124288"/>
-        <c:axId val="69837952"/>
+        <c:axId val="148280832"/>
+        <c:axId val="148128320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="66124288"/>
+        <c:axId val="148280832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7773,7 +7877,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69837952"/>
+        <c:crossAx val="148128320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7781,7 +7885,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69837952"/>
+        <c:axId val="148128320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -7793,7 +7897,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66124288"/>
+        <c:crossAx val="148280832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8173,11 +8277,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="145814016"/>
-        <c:axId val="146210816"/>
+        <c:axId val="143762944"/>
+        <c:axId val="148131200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="145814016"/>
+        <c:axId val="143762944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8186,7 +8290,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146210816"/>
+        <c:crossAx val="148131200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8194,7 +8298,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146210816"/>
+        <c:axId val="148131200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -8206,7 +8310,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145814016"/>
+        <c:crossAx val="143762944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8585,11 +8689,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="145815552"/>
-        <c:axId val="146213120"/>
+        <c:axId val="149567488"/>
+        <c:axId val="148134656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="145815552"/>
+        <c:axId val="149567488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8598,7 +8702,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146213120"/>
+        <c:crossAx val="148134656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8606,7 +8710,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146213120"/>
+        <c:axId val="148134656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -8618,7 +8722,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145815552"/>
+        <c:crossAx val="149567488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8973,11 +9077,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="141268480"/>
-        <c:axId val="146216000"/>
+        <c:axId val="149565440"/>
+        <c:axId val="149734528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="141268480"/>
+        <c:axId val="149565440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8986,7 +9090,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146216000"/>
+        <c:crossAx val="149734528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8994,7 +9098,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146216000"/>
+        <c:axId val="149734528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -9006,7 +9110,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141268480"/>
+        <c:crossAx val="149565440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9361,11 +9465,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="147775488"/>
-        <c:axId val="147243008"/>
+        <c:axId val="150687232"/>
+        <c:axId val="149737408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="147775488"/>
+        <c:axId val="150687232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9374,7 +9478,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147243008"/>
+        <c:crossAx val="149737408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9382,7 +9486,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147243008"/>
+        <c:axId val="149737408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -9394,7 +9498,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147775488"/>
+        <c:crossAx val="150687232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9749,11 +9853,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="147994624"/>
-        <c:axId val="147246464"/>
+        <c:axId val="151726080"/>
+        <c:axId val="149740288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="147994624"/>
+        <c:axId val="151726080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9762,7 +9866,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147246464"/>
+        <c:crossAx val="149740288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9770,7 +9874,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147246464"/>
+        <c:axId val="149740288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -9782,7 +9886,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147994624"/>
+        <c:crossAx val="151726080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10289,11 +10393,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="147996160"/>
-        <c:axId val="147248192"/>
+        <c:axId val="143761920"/>
+        <c:axId val="150906560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="147996160"/>
+        <c:axId val="143761920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10302,7 +10406,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147248192"/>
+        <c:crossAx val="150906560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10310,7 +10414,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147248192"/>
+        <c:axId val="150906560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -10322,7 +10426,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147996160"/>
+        <c:crossAx val="143761920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10793,11 +10897,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="148715008"/>
-        <c:axId val="147250496"/>
+        <c:axId val="150582784"/>
+        <c:axId val="150908864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="148715008"/>
+        <c:axId val="150582784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10806,7 +10910,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147250496"/>
+        <c:crossAx val="150908864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10814,7 +10918,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147250496"/>
+        <c:axId val="150908864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -10826,7 +10930,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148715008"/>
+        <c:crossAx val="150582784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11426,10 +11530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E279"/>
+  <dimension ref="A1:E285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
-      <selection activeCell="J261" sqref="J261"/>
+    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
+      <selection activeCell="F213" sqref="F213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11443,22 +11547,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="60" t="s">
         <v>352</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="61" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
@@ -11488,8 +11592,8 @@
       <c r="A5" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B5" s="17">
-        <v>41549</v>
+      <c r="B5" s="17" t="s">
+        <v>364</v>
       </c>
       <c r="C5" s="17">
         <v>41586</v>
@@ -11506,7 +11610,7 @@
         <v>148</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>344</v>
+        <v>365</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>350</v>
@@ -11547,7 +11651,7 @@
         <v>161</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>346</v>
+        <v>366</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>351</v>
@@ -11590,7 +11694,7 @@
       </c>
       <c r="C11" s="20">
         <f>IF(C$72=0, 0,(C$67+C$68)/C$72)</f>
-        <v>0.66666666666666663</v>
+        <v>0.6</v>
       </c>
       <c r="D11" s="20">
         <f>IF(D$72=0, 0,(D$67+D$68)/D$72)</f>
@@ -11615,7 +11719,7 @@
       </c>
       <c r="D12" s="20">
         <f>IF(D$105=0,0,(D$100+D$101)/D$105)</f>
-        <v>0.875</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="E12" s="20">
         <f>IF(E$105=0,0,(E$100+E$101)/E$105)</f>
@@ -11636,7 +11740,7 @@
       </c>
       <c r="D13" s="20">
         <f>IF(D$121=0, 0, (D$116+D$117)/D$121)</f>
-        <v>1</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="E13" s="20">
         <f>IF(E$121=0, 0, (E$116+E$117)/E$121)</f>
@@ -11674,7 +11778,7 @@
       </c>
       <c r="C15" s="20">
         <f>IF(C$171=0, 0, (C$166+C$167)/C$171)</f>
-        <v>1</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="D15" s="20">
         <f>IF(D$171=0, 0, (D$166+D$167)/D$171)</f>
@@ -11690,20 +11794,20 @@
         <v>196</v>
       </c>
       <c r="B16" s="25">
-        <f>IF(B$232=0, 0, (B$227+B$228)/B$232)</f>
-        <v>0.98</v>
+        <f>IF(B$233=0, 0, (B$228+B$229)/B$233)</f>
+        <v>0.94339622641509435</v>
       </c>
       <c r="C16" s="25">
-        <f>IF(C$232=0, 0, (C$227+C$228)/C$232)</f>
-        <v>0.9</v>
+        <f>IF(C$233=0, 0, (C$228+C$229)/C$233)</f>
+        <v>0.86792452830188682</v>
       </c>
       <c r="D16" s="25">
-        <f>IF(D$232=0, 0, (D$227+D$228)/D$232)</f>
-        <v>0.98</v>
+        <f>IF(D$233=0, 0, (D$228+D$229)/D$233)</f>
+        <v>0.96226415094339623</v>
       </c>
       <c r="E16" s="25">
-        <f>IF(E$232=0, 0, (E$227+E$228)/E$232)</f>
-        <v>0.9</v>
+        <f>IF(E$233=0, 0, (E$228+E$229)/E$233)</f>
+        <v>0.90196078431372551</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -12251,8 +12355,8 @@
       <c r="B59" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C59" s="4" t="s">
-        <v>6</v>
+      <c r="C59" s="53" t="s">
+        <v>7</v>
       </c>
       <c r="D59" s="8" t="s">
         <v>7</v>
@@ -12370,7 +12474,7 @@
       <c r="B66" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C66" s="54" t="s">
+      <c r="C66" s="67" t="s">
         <v>7</v>
       </c>
       <c r="D66" s="31" t="s">
@@ -12390,7 +12494,7 @@
       </c>
       <c r="C67" s="10">
         <f>COUNTIF(C52:C66,"pass")</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D67" s="10">
         <f>COUNTIF(D52:D66,"pass")</f>
@@ -12453,7 +12557,7 @@
       </c>
       <c r="C70" s="12">
         <f>COUNTIF(C52:C66,"Fail")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D70" s="12">
         <f>COUNTIF(D52:D66,"Fail")</f>
@@ -12516,7 +12620,7 @@
       </c>
       <c r="C73" s="6">
         <f>IF(C$72=0, 0,(C$67+C$68)/C$72)</f>
-        <v>0.66666666666666663</v>
+        <v>0.6</v>
       </c>
       <c r="D73" s="6">
         <f>IF(D$72=0, 0,(D$67+D$68)/D$72)</f>
@@ -12833,8 +12937,8 @@
       <c r="C92" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D92" s="4" t="s">
-        <v>6</v>
+      <c r="D92" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="E92" s="57" t="s">
         <v>177</v>
@@ -12973,7 +13077,7 @@
       </c>
       <c r="D100" s="10">
         <f>COUNTIF(D76:D99,"pass")</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E100" s="10">
         <f>COUNTIF(E76:E99,"pass")</f>
@@ -13036,7 +13140,7 @@
       </c>
       <c r="D103" s="12">
         <f>COUNTIF(D76:D99,"Fail")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E103" s="12">
         <f>COUNTIF(E76:E99,"Fail")</f>
@@ -13099,7 +13203,7 @@
       </c>
       <c r="D106" s="6">
         <f>IF(D$105=0,0,(D$100+D$101)/D$105)</f>
-        <v>0.875</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="E106" s="6">
         <f>IF(E$105=0,0,(E$100+E$101)/E$105)</f>
@@ -13225,8 +13329,8 @@
       <c r="C114" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D114" s="4" t="s">
-        <v>6</v>
+      <c r="D114" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="E114" s="4" t="s">
         <v>6</v>
@@ -13263,7 +13367,7 @@
       </c>
       <c r="D116" s="10">
         <f>COUNTIF(D109:D115,"pass")</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E116" s="10">
         <f>COUNTIF(E109:E115,"pass")</f>
@@ -13326,7 +13430,7 @@
       </c>
       <c r="D119" s="12">
         <f>COUNTIF(D109:D115,"Fail")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E119" s="12">
         <f>COUNTIF(E109:E115,"Fail")</f>
@@ -13389,7 +13493,7 @@
       </c>
       <c r="D122" s="6">
         <f>IF(D$121=0, 0, (D$116+D$117)/D$121)</f>
-        <v>1</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="E122" s="6">
         <f>IF(E$121=0, 0, (E$116+E$117)/E$121)</f>
@@ -13955,8 +14059,8 @@
       <c r="B155" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C155" s="4" t="s">
-        <v>6</v>
+      <c r="C155" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="D155" s="4" t="s">
         <v>6</v>
@@ -14145,7 +14249,7 @@
       </c>
       <c r="C166" s="10">
         <f>COUNTIF(C154:C165,"pass")</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D166" s="10">
         <f>COUNTIF(D154:D165,"pass")</f>
@@ -14208,7 +14312,7 @@
       </c>
       <c r="C169" s="12">
         <f>COUNTIF(C154:C165,"Fail")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D169" s="12">
         <f>COUNTIF(D154:D165,"Fail")</f>
@@ -14271,7 +14375,7 @@
       </c>
       <c r="C172" s="6">
         <f>IF(C$171=0, 0, (C$166+C$167)/C$171)</f>
-        <v>1</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="D172" s="6">
         <f>IF(D$171=0, 0, (D$166+D$167)/D$171)</f>
@@ -14364,8 +14468,8 @@
       <c r="B178" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C178" s="4" t="s">
-        <v>6</v>
+      <c r="C178" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="D178" s="4" t="s">
         <v>6</v>
@@ -14605,8 +14709,8 @@
       <c r="C192" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D192" s="38" t="s">
-        <v>140</v>
+      <c r="D192" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="E192" s="8" t="s">
         <v>7</v>
@@ -14659,8 +14763,8 @@
       <c r="D195" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E195" s="4" t="s">
-        <v>6</v>
+      <c r="E195" s="8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
@@ -14707,8 +14811,8 @@
       <c r="C198" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D198" s="4" t="s">
-        <v>6</v>
+      <c r="D198" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="E198" s="4" t="s">
         <v>6</v>
@@ -14749,25 +14853,25 @@
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A201" s="23" t="s">
+      <c r="A201" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B201" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C201" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D201" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E201" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" s="23" t="s">
         <v>255</v>
-      </c>
-      <c r="B201" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C201" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D201" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E201" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A202" s="2" t="s">
-        <v>254</v>
       </c>
       <c r="B202" s="4" t="s">
         <v>6</v>
@@ -14784,7 +14888,7 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B203" s="4" t="s">
         <v>6</v>
@@ -14801,32 +14905,41 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
-        <v>251</v>
+        <v>253</v>
+      </c>
+      <c r="B204" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C204" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D204" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E204" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B205" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C205" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D205" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="B205" s="35" t="s">
+      <c r="B206" s="35" t="s">
         <v>144</v>
-      </c>
-      <c r="C205" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D205" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E205" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A206" s="23" t="s">
-        <v>251</v>
-      </c>
-      <c r="B206" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="C206" s="4" t="s">
         <v>6</v>
@@ -14840,7 +14953,7 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="23" t="s">
-        <v>343</v>
+        <v>251</v>
       </c>
       <c r="B207" s="4" t="s">
         <v>6</v>
@@ -14851,27 +14964,36 @@
       <c r="D207" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E207" s="53" t="s">
-        <v>7</v>
+      <c r="E207" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="23" t="s">
-        <v>358</v>
+        <v>343</v>
+      </c>
+      <c r="B208" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C208" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D208" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="E208" s="53" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A209" s="2" t="s">
-        <v>250</v>
+      <c r="A209" s="23" t="s">
+        <v>358</v>
       </c>
       <c r="B209" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C209" s="8" t="s">
-        <v>7</v>
+      <c r="C209" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="D209" s="4" t="s">
         <v>6</v>
@@ -14882,13 +15004,13 @@
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B210" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C210" s="4" t="s">
-        <v>6</v>
+      <c r="C210" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="D210" s="4" t="s">
         <v>6</v>
@@ -14899,7 +15021,7 @@
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
-        <v>273</v>
+        <v>249</v>
       </c>
       <c r="B211" s="4" t="s">
         <v>6</v>
@@ -14916,41 +15038,41 @@
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B212" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C212" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D212" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E212" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="B212" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C212" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D212" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E212" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A213" s="23" t="s">
+      <c r="B213" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C213" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D213" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E213" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A214" s="23" t="s">
         <v>248</v>
-      </c>
-      <c r="B213" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C213" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D213" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E213" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A214" s="2" t="s">
-        <v>247</v>
       </c>
       <c r="B214" s="4" t="s">
         <v>6</v>
@@ -14967,7 +15089,7 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
-        <v>218</v>
+        <v>247</v>
       </c>
       <c r="B215" s="4" t="s">
         <v>6</v>
@@ -14984,7 +15106,7 @@
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
-        <v>246</v>
+        <v>218</v>
       </c>
       <c r="B216" s="4" t="s">
         <v>6</v>
@@ -15001,7 +15123,7 @@
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="B217" s="4" t="s">
         <v>6</v>
@@ -15018,7 +15140,7 @@
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
-        <v>349</v>
+        <v>237</v>
       </c>
       <c r="B218" s="4" t="s">
         <v>6</v>
@@ -15035,7 +15157,7 @@
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
-        <v>296</v>
+        <v>349</v>
       </c>
       <c r="B219" s="4" t="s">
         <v>6</v>
@@ -15052,7 +15174,7 @@
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>245</v>
+        <v>296</v>
       </c>
       <c r="B220" s="4" t="s">
         <v>6</v>
@@ -15069,7 +15191,7 @@
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B221" s="4" t="s">
         <v>6</v>
@@ -15086,7 +15208,7 @@
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
-        <v>313</v>
+        <v>244</v>
       </c>
       <c r="B222" s="4" t="s">
         <v>6</v>
@@ -15103,7 +15225,7 @@
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
-        <v>238</v>
+        <v>313</v>
       </c>
       <c r="B223" s="4" t="s">
         <v>6</v>
@@ -15120,7 +15242,7 @@
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B224" s="4" t="s">
         <v>6</v>
@@ -15137,247 +15259,251 @@
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B225" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C225" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D225" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E225" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="B225" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C225" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D225" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E225" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A226" s="15" t="s">
+      <c r="B226" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C226" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D226" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E226" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227" s="15" t="s">
         <v>312</v>
       </c>
-      <c r="B226" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C226" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D226" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="E226" s="21" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A227" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B227" s="10">
-        <f>COUNTIF(B$175:B$226,"pass")</f>
-        <v>48</v>
-      </c>
-      <c r="C227" s="10">
-        <f>COUNTIF(C$175:C$226,"pass")</f>
-        <v>45</v>
-      </c>
-      <c r="D227" s="10">
-        <f>COUNTIF(D$175:D$226,"pass")</f>
-        <v>49</v>
-      </c>
-      <c r="E227" s="10">
-        <f>COUNTIF(E$176:E$226,"pass")</f>
-        <v>45</v>
+      <c r="B227" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C227" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D227" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E227" s="21" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B228" s="5">
-        <f>COUNTIF(B$175:B$226,"Ok")</f>
-        <v>1</v>
-      </c>
-      <c r="C228" s="5">
-        <f>COUNTIF(C$175:C$226,"Ok")</f>
-        <v>0</v>
-      </c>
-      <c r="D228" s="5">
-        <f>COUNTIF(D$175:D$226,"Ok")</f>
-        <v>0</v>
-      </c>
-      <c r="E228" s="5">
-        <f>COUNTIF(E$176:E$226,"Ok")</f>
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="B228" s="10">
+        <f>COUNTIF(B$175:B$227,"pass")</f>
+        <v>49</v>
+      </c>
+      <c r="C228" s="10">
+        <f>COUNTIF(C$175:C$227,"pass")</f>
+        <v>46</v>
+      </c>
+      <c r="D228" s="10">
+        <f>COUNTIF(D$175:D$227,"pass")</f>
+        <v>51</v>
+      </c>
+      <c r="E228" s="10">
+        <f>COUNTIF(E$176:E$227,"pass")</f>
+        <v>46</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B229" s="11">
-        <f>COUNTIF(B$175:B$226,"workaround")</f>
-        <v>0</v>
-      </c>
-      <c r="C229" s="11">
-        <f>COUNTIF(C$175:C$226,"workaround")</f>
-        <v>0</v>
-      </c>
-      <c r="D229" s="11">
-        <f>COUNTIF(D$175:D$226,"workaround")</f>
+        <v>143</v>
+      </c>
+      <c r="B229" s="5">
+        <f>COUNTIF(B$175:B$227,"Ok")</f>
         <v>1</v>
       </c>
-      <c r="E229" s="11">
-        <f>COUNTIF(E$176:E$226,"workaround")</f>
+      <c r="C229" s="5">
+        <f>COUNTIF(C$175:C$227,"Ok")</f>
+        <v>0</v>
+      </c>
+      <c r="D229" s="5">
+        <f>COUNTIF(D$175:D$227,"Ok")</f>
+        <v>0</v>
+      </c>
+      <c r="E229" s="5">
+        <f>COUNTIF(E$176:E$227,"Ok")</f>
         <v>0</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B230" s="12">
-        <f>COUNTIF(B175:B226,"Fail")</f>
-        <v>1</v>
-      </c>
-      <c r="C230" s="12">
-        <f>COUNTIF(C175:C226,"Fail")</f>
-        <v>5</v>
-      </c>
-      <c r="D230" s="12">
-        <f>COUNTIF(D175:D226,"Fail")</f>
-        <v>0</v>
-      </c>
-      <c r="E230" s="12">
-        <f>COUNTIF(E176:E226,"Fail")</f>
-        <v>5</v>
+        <v>140</v>
+      </c>
+      <c r="B230" s="11">
+        <f>COUNTIF(B$175:B$227,"workaround")</f>
+        <v>0</v>
+      </c>
+      <c r="C230" s="11">
+        <f>COUNTIF(C$175:C$227,"workaround")</f>
+        <v>0</v>
+      </c>
+      <c r="D230" s="11">
+        <f>COUNTIF(D$175:D$227,"workaround")</f>
+        <v>0</v>
+      </c>
+      <c r="E230" s="11">
+        <f>COUNTIF(E$176:E$227,"workaround")</f>
+        <v>0</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B231" s="2">
-        <f>COUNT(B$179:B$213,"Untested")</f>
-        <v>0</v>
-      </c>
-      <c r="C231" s="2">
-        <f>COUNT(C$179:C$213,"Untested")</f>
-        <v>0</v>
-      </c>
-      <c r="D231" s="2">
-        <f>COUNT(D$179:D$213,"Untested")</f>
-        <v>0</v>
-      </c>
-      <c r="E231" s="2">
-        <f>COUNT(E$179:E$213,"Untested")</f>
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="B231" s="12">
+        <f>COUNTIF(B175:B227,"Fail")</f>
+        <v>3</v>
+      </c>
+      <c r="C231" s="12">
+        <f>COUNTIF(C175:C227,"Fail")</f>
+        <v>7</v>
+      </c>
+      <c r="D231" s="12">
+        <f>COUNTIF(D175:D227,"Fail")</f>
+        <v>2</v>
+      </c>
+      <c r="E231" s="12">
+        <f>COUNTIF(E176:E227,"Fail")</f>
+        <v>5</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B232" s="2">
+        <f>COUNT(B$179:B$214,"Untested")</f>
+        <v>0</v>
+      </c>
+      <c r="C232" s="2">
+        <f>COUNT(C$179:C$214,"Untested")</f>
+        <v>0</v>
+      </c>
+      <c r="D232" s="2">
+        <f>COUNT(D$179:D$214,"Untested")</f>
+        <v>0</v>
+      </c>
+      <c r="E232" s="2">
+        <f>COUNT(E$179:E$214,"Untested")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A233" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B232" s="2">
-        <f>B$227+B$230+B$229+B$231+B$228</f>
-        <v>50</v>
-      </c>
-      <c r="C232" s="2">
-        <f>C$227+C$230+C$229+C$231+C$228</f>
-        <v>50</v>
-      </c>
-      <c r="D232" s="2">
-        <f>D$227+D$230+D$229+D$231+D$228</f>
-        <v>50</v>
-      </c>
-      <c r="E232" s="2">
-        <f>E$227+E$230+E$229+E$231+E$228</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="233" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A233" s="18" t="s">
+      <c r="B233" s="2">
+        <f>B$228+B$231+B$230+B$232+B$229</f>
+        <v>53</v>
+      </c>
+      <c r="C233" s="2">
+        <f>C$228+C$231+C$230+C$232+C$229</f>
+        <v>53</v>
+      </c>
+      <c r="D233" s="2">
+        <f>D$228+D$231+D$230+D$232+D$229</f>
+        <v>53</v>
+      </c>
+      <c r="E233" s="2">
+        <f>E$228+E$231+E$230+E$232+E$229</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A234" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B233" s="6">
-        <f>IF(B$232=0, 0, (B$227+B$228)/B$232)</f>
-        <v>0.98</v>
-      </c>
-      <c r="C233" s="6">
-        <f>IF(C$232=0, 0, (C$227+C$228)/C$232)</f>
-        <v>0.9</v>
-      </c>
-      <c r="D233" s="6">
-        <f>IF(D$232=0, 0, (D$227+D$228)/D$232)</f>
-        <v>0.98</v>
-      </c>
-      <c r="E233" s="6">
-        <f>IF(E$232=0, 0, (E$227+E$228)/E$232)</f>
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="234" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A234" s="13"/>
-      <c r="B234" s="16"/>
-      <c r="C234" s="13"/>
-      <c r="D234" s="13"/>
-      <c r="E234" s="13"/>
-    </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A235" s="19" t="s">
+      <c r="B234" s="6">
+        <f>IF(B$233=0, 0, (B$228+B$229)/B$233)</f>
+        <v>0.94339622641509435</v>
+      </c>
+      <c r="C234" s="6">
+        <f>IF(C$233=0, 0, (C$228+C$229)/C$233)</f>
+        <v>0.86792452830188682</v>
+      </c>
+      <c r="D234" s="6">
+        <f>IF(D$233=0, 0, (D$228+D$229)/D$233)</f>
+        <v>0.96226415094339623</v>
+      </c>
+      <c r="E234" s="6">
+        <f>IF(E$233=0, 0, (E$228+E$229)/E$233)</f>
+        <v>0.90196078431372551</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A235" s="13"/>
+      <c r="B235" s="16"/>
+      <c r="C235" s="13"/>
+      <c r="D235" s="13"/>
+      <c r="E235" s="13"/>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A236" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="B235" s="55" t="s">
+      <c r="B236" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C235" s="56" t="s">
+      <c r="C236" s="56" t="s">
         <v>151</v>
       </c>
-      <c r="D235" s="56" t="s">
+      <c r="D236" s="56" t="s">
         <v>190</v>
       </c>
-      <c r="E235" s="3" t="s">
+      <c r="E236" s="3" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A236" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="B236" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C236" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D236" s="2"/>
-      <c r="E236" s="2"/>
-    </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A237" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="B237" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C237" s="2"/>
+      <c r="A237" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="B237" s="2"/>
+      <c r="C237" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="D237" s="2"/>
       <c r="E237" s="2"/>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B238" s="2"/>
-      <c r="C238" s="4" t="s">
-        <v>6</v>
-      </c>
+        <v>207</v>
+      </c>
+      <c r="B238" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C238" s="2"/>
       <c r="D238" s="2"/>
       <c r="E238" s="2"/>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B239" s="2"/>
       <c r="C239" s="4" t="s">
@@ -15388,7 +15514,7 @@
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B240" s="2"/>
       <c r="C240" s="4" t="s">
@@ -15399,621 +15525,697 @@
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B241" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C241" s="2"/>
+        <v>201</v>
+      </c>
+      <c r="B241" s="2"/>
+      <c r="C241" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="D241" s="2"/>
       <c r="E241" s="2"/>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="B242" s="2"/>
-      <c r="C242" s="4" t="s">
-        <v>6</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="B242" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C242" s="2"/>
       <c r="D242" s="2"/>
       <c r="E242" s="2"/>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="B243" s="4" t="s">
-        <v>6</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="B243" s="2"/>
       <c r="C243" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D243" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="D243" s="2"/>
       <c r="E243" s="2"/>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B244" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C244" s="2"/>
-      <c r="D244" s="2"/>
+      <c r="C244" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D244" s="8" t="s">
+        <v>7</v>
+      </c>
       <c r="E244" s="2"/>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="B245" s="2"/>
-      <c r="C245" s="4" t="s">
-        <v>6</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="B245" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C245" s="2"/>
       <c r="D245" s="2"/>
       <c r="E245" s="2"/>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="B246" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C246" s="2"/>
+        <v>274</v>
+      </c>
+      <c r="B246" s="2"/>
+      <c r="C246" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="D246" s="2"/>
       <c r="E246" s="2"/>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="B247" s="2"/>
-      <c r="C247" s="4" t="s">
-        <v>6</v>
-      </c>
+        <v>205</v>
+      </c>
+      <c r="B247" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C247" s="2"/>
       <c r="D247" s="2"/>
       <c r="E247" s="2"/>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A248" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="B248" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C248" s="15"/>
-      <c r="D248" s="15"/>
-      <c r="E248" s="15"/>
+      <c r="A248" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B248" s="2"/>
+      <c r="C248" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D248" s="2"/>
+      <c r="E248" s="2"/>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B249" s="10">
-        <f>COUNTIF(B236:B248,"pass")</f>
-        <v>7</v>
-      </c>
-      <c r="C249" s="10">
-        <f>COUNTIF(C236:C248,"pass")</f>
-        <v>8</v>
-      </c>
-      <c r="D249" s="10">
-        <f>COUNTIF(D236:D248,"pass")</f>
-        <v>0</v>
-      </c>
-      <c r="E249" s="10">
-        <f>COUNTIF(E236:E248,"pass")</f>
-        <v>0</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="B249" s="2"/>
+      <c r="C249" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D249" s="2"/>
+      <c r="E249" s="2"/>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B250" s="5">
-        <f>COUNTIF(B236:B248,"Ok")</f>
-        <v>0</v>
-      </c>
-      <c r="C250" s="5">
-        <f>COUNTIF(C236:C248,"Ok")</f>
-        <v>0</v>
-      </c>
-      <c r="D250" s="5">
-        <f>COUNTIF(D236:D248,"Ok")</f>
-        <v>0</v>
-      </c>
-      <c r="E250" s="5">
-        <f>COUNTIF(E236:E248,"Ok")</f>
-        <v>0</v>
-      </c>
+        <v>199</v>
+      </c>
+      <c r="B250" s="2"/>
+      <c r="C250" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D250" s="2"/>
+      <c r="E250" s="2"/>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A251" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B251" s="11">
-        <f>COUNTIF(B236:B248,"workaround")</f>
-        <v>0</v>
-      </c>
-      <c r="C251" s="11">
-        <f>COUNTIF(C236:C248,"workaround")</f>
-        <v>0</v>
-      </c>
-      <c r="D251" s="11">
-        <f>COUNTIF(D236:D248,"workaround")</f>
-        <v>0</v>
-      </c>
-      <c r="E251" s="11">
-        <f>COUNTIF(E236:E248,"workaround")</f>
-        <v>0</v>
-      </c>
+      <c r="A251" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="B251" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C251" s="2"/>
+      <c r="D251" s="2"/>
+      <c r="E251" s="2"/>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B252" s="12">
-        <f>COUNTIF(B236:B248,"Fail")</f>
-        <v>0</v>
-      </c>
-      <c r="C252" s="12">
-        <f>COUNTIF(C236:C248,"Fail")</f>
-        <v>0</v>
-      </c>
-      <c r="D252" s="12">
-        <f>COUNTIF(D236:D248,"Fail")</f>
-        <v>1</v>
-      </c>
-      <c r="E252" s="12">
-        <f>COUNTIF(E236:E248,"Fail")</f>
-        <v>0</v>
-      </c>
+        <v>362</v>
+      </c>
+      <c r="B252" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C252" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D252" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E252" s="2"/>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B253" s="2">
-        <f>COUNT(B236:B248,"Untested")</f>
-        <v>0</v>
-      </c>
-      <c r="C253" s="2">
-        <f>COUNT(C236:C248,"Untested")</f>
-        <v>0</v>
-      </c>
-      <c r="D253" s="2">
-        <f>COUNT(D236:D248,"Untested")</f>
-        <v>0</v>
-      </c>
-      <c r="E253" s="2">
-        <f>COUNT(E236:E248,"Untested")</f>
-        <v>0</v>
-      </c>
+        <v>276</v>
+      </c>
+      <c r="B253" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C253" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D253" s="2"/>
+      <c r="E253" s="2"/>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B254" s="2">
-        <f>B249+B252+B251+B253+B250</f>
+        <v>361</v>
+      </c>
+      <c r="B254" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C254" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D254" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E254" s="2"/>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A255" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="B255" s="59">
+        <f>COUNTIF(B237:B254,"pass")</f>
+        <v>9</v>
+      </c>
+      <c r="C255" s="59">
+        <f t="shared" ref="C255:E255" si="3">COUNTIF(C237:C254,"pass")</f>
+        <v>13</v>
+      </c>
+      <c r="D255" s="59">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E255" s="59">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A256" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B256" s="5">
+        <f>COUNTIF(B237:B254,"Ok")</f>
+        <v>0</v>
+      </c>
+      <c r="C256" s="5">
+        <f t="shared" ref="C256:E256" si="4">COUNTIF(C237:C254,"Ok")</f>
+        <v>0</v>
+      </c>
+      <c r="D256" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E256" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A257" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B257" s="11">
+        <f>COUNTIF(B237:B254,"workaround")</f>
+        <v>0</v>
+      </c>
+      <c r="C257" s="11">
+        <f>COUNTIF(C239:C253,"workaround")</f>
+        <v>0</v>
+      </c>
+      <c r="D257" s="11">
+        <f>COUNTIF(D239:D253,"workaround")</f>
+        <v>0</v>
+      </c>
+      <c r="E257" s="11">
+        <f>COUNTIF(E239:E253,"workaround")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A258" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C254" s="2">
-        <f>C249+C252+C251+C253+C250</f>
-        <v>8</v>
-      </c>
-      <c r="D254" s="2">
-        <f>D249+D252+D251+D253+D250</f>
+      <c r="B258" s="12">
+        <f>COUNTIF(B237:B254,"Fail")</f>
+        <v>0</v>
+      </c>
+      <c r="C258" s="12">
+        <f t="shared" ref="C258:E258" si="5">COUNTIF(C237:C254,"Fail")</f>
+        <v>0</v>
+      </c>
+      <c r="D258" s="12">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="E254" s="2">
-        <f>E249+E252+E251+E253+E250</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="255" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A255" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B255" s="6">
-        <f>IF(B$254=0, 0, (B$249+B$250)/B$254)</f>
-        <v>1</v>
-      </c>
-      <c r="C255" s="6">
-        <f>IF(C$254=0, 0, (C$249+C$250)/C$254)</f>
-        <v>1</v>
-      </c>
-      <c r="D255" s="6">
-        <f>IF(D$254=0, 0, (D$249+D$250)/D$254)</f>
-        <v>0</v>
-      </c>
-      <c r="E255" s="6">
-        <f>IF(E$254=0, 0, (E$249+E$250)/E$254)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="256" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A256" s="13"/>
-      <c r="B256" s="13"/>
-      <c r="C256" s="13"/>
-      <c r="D256" s="13"/>
-      <c r="E256" s="13"/>
-    </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A257" s="15" t="s">
-        <v>354</v>
-      </c>
-      <c r="B257" s="15"/>
-      <c r="C257" s="15"/>
-      <c r="D257" s="15"/>
-      <c r="E257" s="15"/>
-    </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A258" s="28" t="s">
-        <v>355</v>
-      </c>
-      <c r="B258" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="C258" s="28"/>
-      <c r="D258" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E258" s="28"/>
+      <c r="E258" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B259" s="10">
-        <f>COUNTIF(B258,"pass")</f>
-        <v>1</v>
-      </c>
-      <c r="C259" s="10">
-        <f>COUNTIF(C258,"pass")</f>
-        <v>0</v>
-      </c>
-      <c r="D259" s="10">
-        <f>COUNTIF(D258,"pass")</f>
-        <v>1</v>
-      </c>
-      <c r="E259" s="10">
-        <f>COUNTIF(E258,"pass")</f>
+        <v>145</v>
+      </c>
+      <c r="B259" s="2">
+        <f>COUNT(B237:B254,"Untested")</f>
+        <v>0</v>
+      </c>
+      <c r="C259" s="2">
+        <f t="shared" ref="C259:E259" si="6">COUNT(C237:C254,"Untested")</f>
+        <v>0</v>
+      </c>
+      <c r="D259" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E259" s="2">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B260" s="2">
+        <f>B255+B258+B257+B259+B256</f>
+        <v>9</v>
+      </c>
+      <c r="C260" s="2">
+        <f>C255+C258+C257+C259+C256</f>
+        <v>13</v>
+      </c>
+      <c r="D260" s="2">
+        <f>D255+D258+D257+D259+D256</f>
+        <v>3</v>
+      </c>
+      <c r="E260" s="2">
+        <f>E255+E258+E257+E259+E256</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A261" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B261" s="6">
+        <f>IF(B$260=0, 0, (B$255+B$256)/B$260)</f>
+        <v>1</v>
+      </c>
+      <c r="C261" s="6">
+        <f>IF(C$260=0, 0, (C$255+C$256)/C$260)</f>
+        <v>1</v>
+      </c>
+      <c r="D261" s="6">
+        <f>IF(D$260=0, 0, (D$255+D$256)/D$260)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E261" s="6">
+        <f>IF(E$260=0, 0, (E$255+E$256)/E$260)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A262" s="13"/>
+      <c r="B262" s="13"/>
+      <c r="C262" s="13"/>
+      <c r="D262" s="13"/>
+      <c r="E262" s="13"/>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A263" s="15" t="s">
+        <v>354</v>
+      </c>
+      <c r="B263" s="15"/>
+      <c r="C263" s="15"/>
+      <c r="D263" s="15"/>
+      <c r="E263" s="15"/>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A264" s="28" t="s">
+        <v>355</v>
+      </c>
+      <c r="B264" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C264" s="28"/>
+      <c r="D264" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E264" s="28"/>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A265" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B265" s="10">
+        <f>COUNTIF(B264,"pass")</f>
+        <v>1</v>
+      </c>
+      <c r="C265" s="10">
+        <f>COUNTIF(C264,"pass")</f>
+        <v>0</v>
+      </c>
+      <c r="D265" s="10">
+        <f>COUNTIF(D264,"pass")</f>
+        <v>1</v>
+      </c>
+      <c r="E265" s="10">
+        <f>COUNTIF(E264,"pass")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A266" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B260" s="5">
-        <f>COUNTIF(B258,"Ok")</f>
-        <v>0</v>
-      </c>
-      <c r="C260" s="5">
-        <f>COUNTIF(C258,"Ok")</f>
-        <v>0</v>
-      </c>
-      <c r="D260" s="5">
-        <f>COUNTIF(D258,"Ok")</f>
-        <v>0</v>
-      </c>
-      <c r="E260" s="5">
-        <f>COUNTIF(E258,"Ok")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A261" s="2" t="s">
+      <c r="B266" s="5">
+        <f>COUNTIF(B264,"Ok")</f>
+        <v>0</v>
+      </c>
+      <c r="C266" s="5">
+        <f>COUNTIF(C264,"Ok")</f>
+        <v>0</v>
+      </c>
+      <c r="D266" s="5">
+        <f>COUNTIF(D264,"Ok")</f>
+        <v>0</v>
+      </c>
+      <c r="E266" s="5">
+        <f>COUNTIF(E264,"Ok")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A267" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B261" s="11">
-        <f>COUNTIF(B258,"workaround")</f>
-        <v>0</v>
-      </c>
-      <c r="C261" s="11">
-        <f>COUNTIF(C258,"workaround")</f>
-        <v>0</v>
-      </c>
-      <c r="D261" s="11">
-        <f>COUNTIF(D258,"workaround")</f>
-        <v>0</v>
-      </c>
-      <c r="E261" s="11">
-        <f>COUNTIF(E258,"workaround")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A262" s="2" t="s">
+      <c r="B267" s="11">
+        <f>COUNTIF(B264,"workaround")</f>
+        <v>0</v>
+      </c>
+      <c r="C267" s="11">
+        <f>COUNTIF(C264,"workaround")</f>
+        <v>0</v>
+      </c>
+      <c r="D267" s="11">
+        <f>COUNTIF(D264,"workaround")</f>
+        <v>0</v>
+      </c>
+      <c r="E267" s="11">
+        <f>COUNTIF(E264,"workaround")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A268" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B262" s="12">
-        <f>COUNTIF(B258,"Fail")</f>
-        <v>0</v>
-      </c>
-      <c r="C262" s="12">
-        <f>COUNTIF(C258,"Fail")</f>
-        <v>0</v>
-      </c>
-      <c r="D262" s="12">
-        <f>COUNTIF(D258,"Fail")</f>
-        <v>0</v>
-      </c>
-      <c r="E262" s="12">
-        <f>COUNTIF(E258,"Fail")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A263" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B263" s="2">
-        <f>COUNT(B258,"Untested")</f>
-        <v>0</v>
-      </c>
-      <c r="C263" s="2">
-        <f>COUNT(C258,"Untested")</f>
-        <v>0</v>
-      </c>
-      <c r="D263" s="2">
-        <f>COUNT(D258,"Untested")</f>
-        <v>0</v>
-      </c>
-      <c r="E263" s="2">
-        <f>COUNT(E258,"Untested")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A264" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B264" s="2">
-        <f>B259+B262+B261+B263+B260</f>
-        <v>1</v>
-      </c>
-      <c r="C264" s="2">
-        <f>C259+C262+C261+C263+C260</f>
-        <v>0</v>
-      </c>
-      <c r="D264" s="2">
-        <f>D259+D262+D261+D263+D260</f>
-        <v>1</v>
-      </c>
-      <c r="E264" s="2">
-        <f>E259+E262+E261+E263+E260</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="265" spans="1:5" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A265" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B265" s="6">
-        <f>IF(B$274=0, 0, (B$269+B$270)/B$274)</f>
-        <v>1</v>
-      </c>
-      <c r="C265" s="6">
-        <f>IF(C$274=0, 0, (C$269+C$270)/C$274)</f>
-        <v>0</v>
-      </c>
-      <c r="D265" s="6">
-        <f>IF(D$274=0, 0, (D$269+D$270)/D$274)</f>
-        <v>1</v>
-      </c>
-      <c r="E265" s="6">
-        <f>IF(E$274=0, 0, (E$269+E$270)/E$274)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="266" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A266" s="13"/>
-      <c r="B266" s="13"/>
-      <c r="C266" s="13"/>
-      <c r="D266" s="13"/>
-      <c r="E266" s="13"/>
-    </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A267" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B267" s="15"/>
-      <c r="C267" s="15"/>
-      <c r="D267" s="15"/>
-      <c r="E267" s="15"/>
-    </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A268" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="B268" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="C268" s="28"/>
-      <c r="D268" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E268" s="28"/>
+      <c r="B268" s="12">
+        <f>COUNTIF(B264,"Fail")</f>
+        <v>0</v>
+      </c>
+      <c r="C268" s="12">
+        <f>COUNTIF(C264,"Fail")</f>
+        <v>0</v>
+      </c>
+      <c r="D268" s="12">
+        <f>COUNTIF(D264,"Fail")</f>
+        <v>0</v>
+      </c>
+      <c r="E268" s="12">
+        <f>COUNTIF(E264,"Fail")</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B269" s="10">
-        <f>COUNTIF(B268,"pass")</f>
-        <v>1</v>
-      </c>
-      <c r="C269" s="10">
-        <f>COUNTIF(C268,"pass")</f>
-        <v>0</v>
-      </c>
-      <c r="D269" s="10">
-        <f>COUNTIF(D268,"pass")</f>
-        <v>1</v>
-      </c>
-      <c r="E269" s="10">
-        <f>COUNTIF(E268,"pass")</f>
+        <v>145</v>
+      </c>
+      <c r="B269" s="2">
+        <f>COUNT(B264,"Untested")</f>
+        <v>0</v>
+      </c>
+      <c r="C269" s="2">
+        <f>COUNT(C264,"Untested")</f>
+        <v>0</v>
+      </c>
+      <c r="D269" s="2">
+        <f>COUNT(D264,"Untested")</f>
+        <v>0</v>
+      </c>
+      <c r="E269" s="2">
+        <f>COUNT(E264,"Untested")</f>
         <v>0</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B270" s="2">
+        <f>B265+B268+B267+B269+B266</f>
+        <v>1</v>
+      </c>
+      <c r="C270" s="2">
+        <f>C265+C268+C267+C269+C266</f>
+        <v>0</v>
+      </c>
+      <c r="D270" s="2">
+        <f>D265+D268+D267+D269+D266</f>
+        <v>1</v>
+      </c>
+      <c r="E270" s="2">
+        <f>E265+E268+E267+E269+E266</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A271" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B271" s="6">
+        <f>IF(B$280=0, 0, (B$275+B$276)/B$280)</f>
+        <v>1</v>
+      </c>
+      <c r="C271" s="6">
+        <f>IF(C$280=0, 0, (C$275+C$276)/C$280)</f>
+        <v>0</v>
+      </c>
+      <c r="D271" s="6">
+        <f>IF(D$280=0, 0, (D$275+D$276)/D$280)</f>
+        <v>1</v>
+      </c>
+      <c r="E271" s="6">
+        <f>IF(E$280=0, 0, (E$275+E$276)/E$280)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A272" s="13"/>
+      <c r="B272" s="13"/>
+      <c r="C272" s="13"/>
+      <c r="D272" s="13"/>
+      <c r="E272" s="13"/>
+    </row>
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A273" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B273" s="15"/>
+      <c r="C273" s="15"/>
+      <c r="D273" s="15"/>
+      <c r="E273" s="15"/>
+    </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A274" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B274" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C274" s="28"/>
+      <c r="D274" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E274" s="28"/>
+    </row>
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A275" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B275" s="10">
+        <f>COUNTIF(B274,"pass")</f>
+        <v>1</v>
+      </c>
+      <c r="C275" s="10">
+        <f>COUNTIF(C274,"pass")</f>
+        <v>0</v>
+      </c>
+      <c r="D275" s="10">
+        <f>COUNTIF(D274,"pass")</f>
+        <v>1</v>
+      </c>
+      <c r="E275" s="10">
+        <f>COUNTIF(E274,"pass")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A276" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B270" s="5">
-        <f>COUNTIF(B268,"Ok")</f>
-        <v>0</v>
-      </c>
-      <c r="C270" s="5">
-        <f>COUNTIF(C268,"Ok")</f>
-        <v>0</v>
-      </c>
-      <c r="D270" s="5">
-        <f>COUNTIF(D268,"Ok")</f>
-        <v>0</v>
-      </c>
-      <c r="E270" s="5">
-        <f>COUNTIF(E268,"Ok")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A271" s="2" t="s">
+      <c r="B276" s="5">
+        <f>COUNTIF(B274,"Ok")</f>
+        <v>0</v>
+      </c>
+      <c r="C276" s="5">
+        <f>COUNTIF(C274,"Ok")</f>
+        <v>0</v>
+      </c>
+      <c r="D276" s="5">
+        <f>COUNTIF(D274,"Ok")</f>
+        <v>0</v>
+      </c>
+      <c r="E276" s="5">
+        <f>COUNTIF(E274,"Ok")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A277" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B271" s="11">
-        <f>COUNTIF(B268,"workaround")</f>
-        <v>0</v>
-      </c>
-      <c r="C271" s="11">
-        <f>COUNTIF(C268,"workaround")</f>
-        <v>0</v>
-      </c>
-      <c r="D271" s="11">
-        <f>COUNTIF(D268,"workaround")</f>
-        <v>0</v>
-      </c>
-      <c r="E271" s="11">
-        <f>COUNTIF(E268,"workaround")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A272" s="2" t="s">
+      <c r="B277" s="11">
+        <f>COUNTIF(B274,"workaround")</f>
+        <v>0</v>
+      </c>
+      <c r="C277" s="11">
+        <f>COUNTIF(C274,"workaround")</f>
+        <v>0</v>
+      </c>
+      <c r="D277" s="11">
+        <f>COUNTIF(D274,"workaround")</f>
+        <v>0</v>
+      </c>
+      <c r="E277" s="11">
+        <f>COUNTIF(E274,"workaround")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A278" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B272" s="12">
-        <f>COUNTIF(B268,"Fail")</f>
-        <v>0</v>
-      </c>
-      <c r="C272" s="12">
-        <f>COUNTIF(C268,"Fail")</f>
-        <v>0</v>
-      </c>
-      <c r="D272" s="12">
-        <f>COUNTIF(D268,"Fail")</f>
-        <v>0</v>
-      </c>
-      <c r="E272" s="12">
-        <f>COUNTIF(E268,"Fail")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A273" s="2" t="s">
+      <c r="B278" s="12">
+        <f>COUNTIF(B274,"Fail")</f>
+        <v>0</v>
+      </c>
+      <c r="C278" s="12">
+        <f>COUNTIF(C274,"Fail")</f>
+        <v>0</v>
+      </c>
+      <c r="D278" s="12">
+        <f>COUNTIF(D274,"Fail")</f>
+        <v>0</v>
+      </c>
+      <c r="E278" s="12">
+        <f>COUNTIF(E274,"Fail")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A279" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B273" s="2">
-        <f>COUNT(B268,"Untested")</f>
-        <v>0</v>
-      </c>
-      <c r="C273" s="2">
-        <f>COUNT(C268,"Untested")</f>
-        <v>0</v>
-      </c>
-      <c r="D273" s="2">
-        <f>COUNT(D268,"Untested")</f>
-        <v>0</v>
-      </c>
-      <c r="E273" s="2">
-        <f>COUNT(E268,"Untested")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A274" s="2" t="s">
+      <c r="B279" s="2">
+        <f>COUNT(B274,"Untested")</f>
+        <v>0</v>
+      </c>
+      <c r="C279" s="2">
+        <f>COUNT(C274,"Untested")</f>
+        <v>0</v>
+      </c>
+      <c r="D279" s="2">
+        <f>COUNT(D274,"Untested")</f>
+        <v>0</v>
+      </c>
+      <c r="E279" s="2">
+        <f>COUNT(E274,"Untested")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A280" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B274" s="2">
-        <f>B269+B272+B271+B273+B270</f>
+      <c r="B280" s="2">
+        <f>B275+B278+B277+B279+B276</f>
         <v>1</v>
       </c>
-      <c r="C274" s="2">
-        <f>C269+C272+C271+C273+C270</f>
-        <v>0</v>
-      </c>
-      <c r="D274" s="2">
-        <f>D269+D272+D271+D273+D270</f>
+      <c r="C280" s="2">
+        <f>C275+C278+C277+C279+C276</f>
+        <v>0</v>
+      </c>
+      <c r="D280" s="2">
+        <f>D275+D278+D277+D279+D276</f>
         <v>1</v>
       </c>
-      <c r="E274" s="2">
-        <f>E269+E272+E271+E273+E270</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="275" spans="1:5" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A275" s="18" t="s">
+      <c r="E280" s="2">
+        <f>E275+E278+E277+E279+E276</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A281" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B275" s="6">
-        <f>IF(B$274=0, 0, (B$269+B$270)/B$274)</f>
+      <c r="B281" s="6">
+        <f>IF(B$280=0, 0, (B$275+B$276)/B$280)</f>
         <v>1</v>
       </c>
-      <c r="C275" s="6">
-        <f>IF(C$274=0, 0, (C$269+C$270)/C$274)</f>
-        <v>0</v>
-      </c>
-      <c r="D275" s="6">
-        <f>IF(D$274=0, 0, (D$269+D$270)/D$274)</f>
+      <c r="C281" s="6">
+        <f>IF(C$280=0, 0, (C$275+C$276)/C$280)</f>
+        <v>0</v>
+      </c>
+      <c r="D281" s="6">
+        <f>IF(D$280=0, 0, (D$275+D$276)/D$280)</f>
         <v>1</v>
       </c>
-      <c r="E275" s="6">
-        <f>IF(E$274=0, 0, (E$269+E$270)/E$274)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="276" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A276" s="1"/>
-      <c r="B276" s="1"/>
-      <c r="C276" s="1"/>
-      <c r="D276" s="1"/>
-      <c r="E276" s="1"/>
-    </row>
-    <row r="277" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B277" s="20"/>
-      <c r="C277" s="20"/>
-      <c r="D277" s="20"/>
-      <c r="E277" s="20"/>
-    </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A278" s="2"/>
-      <c r="B278" s="20"/>
-      <c r="C278" s="20"/>
-      <c r="D278" s="20"/>
-      <c r="E278" s="20"/>
-    </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A279" s="2"/>
-      <c r="B279" s="2"/>
-      <c r="C279" s="2"/>
-      <c r="D279" s="2"/>
-      <c r="E279" s="2"/>
+      <c r="E281" s="6">
+        <f>IF(E$280=0, 0, (E$275+E$276)/E$280)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A282" s="1"/>
+      <c r="B282" s="1"/>
+      <c r="C282" s="1"/>
+      <c r="D282" s="1"/>
+      <c r="E282" s="1"/>
+    </row>
+    <row r="283" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B283" s="20"/>
+      <c r="C283" s="20"/>
+      <c r="D283" s="20"/>
+      <c r="E283" s="20"/>
+    </row>
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A284" s="2"/>
+      <c r="B284" s="20"/>
+      <c r="C284" s="20"/>
+      <c r="D284" s="20"/>
+      <c r="E284" s="20"/>
+    </row>
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A285" s="2"/>
+      <c r="B285" s="2"/>
+      <c r="C285" s="2"/>
+      <c r="D285" s="2"/>
+      <c r="E285" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -16050,22 +16252,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="60" t="s">
         <v>345</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="61" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
@@ -20343,22 +20545,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="60" t="s">
         <v>332</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="61" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
@@ -24619,22 +24821,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="60" t="s">
         <v>330</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="61" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
@@ -28618,22 +28820,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="60" t="s">
         <v>318</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="61" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
@@ -32617,22 +32819,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="60" t="s">
         <v>197</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="61" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
@@ -36617,26 +36819,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="60" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="61" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
@@ -36651,18 +36853,18 @@
       <c r="A4" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B4" s="61" t="s">
+      <c r="B4" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="62" t="s">
+      <c r="C4" s="63"/>
+      <c r="D4" s="64" t="s">
         <v>151</v>
       </c>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62" t="s">
+      <c r="E4" s="64"/>
+      <c r="F4" s="64" t="s">
         <v>150</v>
       </c>
-      <c r="G4" s="62"/>
+      <c r="G4" s="64"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -41964,26 +42166,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="60" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="61" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
@@ -41998,18 +42200,18 @@
       <c r="A4" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B4" s="61" t="s">
+      <c r="B4" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="62" t="s">
+      <c r="C4" s="63"/>
+      <c r="D4" s="64" t="s">
         <v>151</v>
       </c>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62" t="s">
+      <c r="E4" s="64"/>
+      <c r="F4" s="64" t="s">
         <v>150</v>
       </c>
-      <c r="G4" s="62"/>
+      <c r="G4" s="64"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -46670,14 +46872,14 @@
       <c r="A1" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="64" t="s">
+      <c r="C1" s="65"/>
+      <c r="D1" s="66" t="s">
         <v>151</v>
       </c>
-      <c r="E1" s="64"/>
+      <c r="E1" s="66"/>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">

</xml_diff>

<commit_message>
Added post, picture 07, driver status
</commit_message>
<xml_diff>
--- a/doc/OpenGL status.xlsx
+++ b/doc/OpenGL status.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="0" windowWidth="12480" windowHeight="15210"/>
+    <workbookView xWindow="45" yWindow="0" windowWidth="13350" windowHeight="18480"/>
   </bookViews>
   <sheets>
     <sheet name="2014-02" sheetId="10" r:id="rId1"/>
@@ -27,34 +27,6 @@
     <author>Groove</author>
   </authors>
   <commentList>
-    <comment ref="B39" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Doesn't support const expression arithmetic: C1154: non constant expression in layout value</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B53" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Object labels not used in the debug output log.</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="C53" authorId="0">
       <text>
         <r>
@@ -110,20 +82,6 @@
             <family val="2"/>
           </rPr>
           <t>Generate a Syntax error: "layout" parse error</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B58" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Allows cast with precision qualifiers</t>
         </r>
       </text>
     </comment>
@@ -225,20 +183,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="B86" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Structure for vertex inputs supported</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="C89" authorId="0">
       <text>
         <r>
@@ -312,20 +256,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="E110" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>GLSL error: "'flat': syntax error syntax error"</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="E111" authorId="0">
       <text>
         <r>
@@ -390,7 +320,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Require glDrawBuffer(GL_NONE) before glCheckFramebuffer otherwise the implementation generates an OpenGL error
 </t>
@@ -408,20 +338,6 @@
             <family val="2"/>
           </rPr>
           <t>Doesn't render the shadow</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E132" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Return the GLSL error: "Invalid use of layout 'stream'.</t>
         </r>
       </text>
     </comment>
@@ -453,20 +369,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="E140" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>LOD query doesn't work</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B142" authorId="0">
       <text>
         <r>
@@ -495,20 +397,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="E142" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Allows to pass a copy of a varying to interpolateAtOffset</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B143" authorId="0">
       <text>
         <r>
@@ -520,36 +408,6 @@
             <family val="2"/>
           </rPr>
           <t>EXT_transform_feedback extension string missing</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B144" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">layout(triangles) in; declaration is required by the specification but the implementation doesn't requires it.
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C144" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">layout(triangles) in; declaration is required by the specification but the implementation doesn't requires it.
-</t>
         </r>
       </text>
     </comment>
@@ -567,7 +425,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E163" authorId="0">
+    <comment ref="E186" authorId="0">
       <text>
         <r>
           <rPr>
@@ -576,21 +434,6 @@
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Doesn't support RGB10A2 texture format correctly. Nothing rendered.
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E186" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
           </rPr>
           <t>Doesn't display the quad</t>
         </r>
@@ -604,7 +447,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Generates a GL_FRAMEBUFFER_INCOMPLETE_DRAW_BUFFER error
 </t>
@@ -619,7 +462,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Generates a GL_FRAMEBUFFER_INCOMPLETE_DRAW_BUFFER error
 </t>
@@ -634,7 +477,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Blit of integer multisample texture with even a single sample per texel doesn't work.</t>
         </r>
@@ -648,7 +491,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>The driver doesn't output vec4(0, 0, 0, 1) when the resolved interger color buffer is incomplete</t>
         </r>
@@ -662,7 +505,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Render a black screen</t>
         </r>
@@ -676,7 +519,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Require glDrawBuffer(GL_NONE) before glCheckFramebuffer otherwise the implementation generates an OpenGL error
 </t>
@@ -691,23 +534,9 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Generate an invalid operation error when on shadow rendering draw call.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E196" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Clearing a FBO bigger than the window dimentions generate unclear bands</t>
         </r>
       </text>
     </comment>
@@ -719,7 +548,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>"lowp int Count = lowp int(COUNT);" should generate an error.
 The valid form is:
@@ -735,7 +564,23 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+          </rPr>
+          <t>"lowp int Count = lowp int(COUNT);" should generate an error.
+The valid form is:
+"lowp int Count = int(COUNT);"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E198" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>"lowp int Count = lowp int(COUNT);" should generate an error.
 The valid form is:
@@ -751,7 +596,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>NVIDIA compiler aspects a structure for the vertex input interface, This is not allowed, it would be nice to have an extension for it.</t>
         </r>
@@ -765,11 +610,9 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
-          <t xml:space="preserve">glClearBufferfv is always performed, even is the condition fails.
-OpenGL 4.3 - 10.10 Conditional Rendering:
-Doesn't generate an GLSL compiler error when geometry shader input layout qualifier is missing
+          <t xml:space="preserve">layout(triangles) in; declaration is required by the specification but the implementation doesn't requires it.
 </t>
         </r>
       </text>
@@ -782,11 +625,9 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
-          <t xml:space="preserve">glClearBufferfv is always performed, even is the condition fails.
-OpenGL 4.3 - 10.10 Conditional Rendering:
-Doesn't generate an GLSL compiler error when geometry shader input layout qualifier is missing
+          <t xml:space="preserve">layout(triangles) in; declaration is required by the specification but the implementation doesn't requires it.
 </t>
         </r>
       </text>
@@ -805,20 +646,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="E208" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Deleting shader object after being attached lead to invalid operations error generated when the program pop the stack</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="C210" authorId="0">
       <text>
         <r>
@@ -827,7 +654,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">glClearBufferfv is always performed, even is the condition fails.
 OpenGL 4.3 - 10.10 Conditional Rendering:
@@ -859,7 +686,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>"The internal format of the texture arrays is integer (see table 3.12), and either the magniﬁcation ﬁlter is not NEAREST, or the miniﬁcation ﬁlter is neither NEAREST nor NEAREST_MIPMAP_NEAREST."
 Other implementation doesn't have this requirement</t>
@@ -1268,7 +1095,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Require glDrawBuffer(GL_NONE) before glCheckFramebuffer otherwise the implementation generates an OpenGL error
 </t>
@@ -1482,7 +1309,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Fixed in this drivers</t>
         </r>
@@ -1496,7 +1323,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Doesn't display the quad</t>
         </r>
@@ -1510,7 +1337,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Generates a GL_FRAMEBUFFER_INCOMPLETE_DRAW_BUFFER error
 </t>
@@ -1525,7 +1352,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Generates a GL_FRAMEBUFFER_INCOMPLETE_DRAW_BUFFER error
 </t>
@@ -1540,7 +1367,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Blit of integer multisample texture with even a single sample per texel doesn't work.</t>
         </r>
@@ -1568,7 +1395,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Render a black screen</t>
         </r>
@@ -1582,7 +1409,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Require glDrawBuffer(GL_NONE) before glCheckFramebuffer otherwise the implementation generates an OpenGL error
 </t>
@@ -1597,7 +1424,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Clearing a FBO bigger than the window dimentions generate unclear bands</t>
         </r>
@@ -1625,7 +1452,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Deleting shader object after being attached lead to invalid operations error generated when the program pop the stack</t>
         </r>
@@ -1639,7 +1466,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">glClearBufferfv is always performed, even is the condition fails.
 OpenGL 4.3 - 10.10 Conditional Rendering:
@@ -1671,7 +1498,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>"The internal format of the texture arrays is integer (see table 3.12), and either the magniﬁcation ﬁlter is not NEAREST, or the miniﬁcation ﬁlter is neither NEAREST nor NEAREST_MIPMAP_NEAREST."
 Other implementation doesn't have this requirement</t>
@@ -2024,7 +1851,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Fixed in this drivers</t>
         </r>
@@ -2066,7 +1893,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">The depth test can't be enable
 </t>
@@ -2095,7 +1922,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Clearing a FBO failed</t>
         </r>
@@ -2109,7 +1936,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Generates a GL_FRAMEBUFFER_INCOMPLETE_DRAW_BUFFER error
 </t>
@@ -2124,7 +1951,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Generates a GL_FRAMEBUFFER_INCOMPLETE_DRAW_BUFFER error
 </t>
@@ -2167,7 +1994,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Blit of integer multisample texture with even a single sample per texel doesn't work.</t>
         </r>
@@ -2181,7 +2008,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Blit of integer multisample texture with even a single sample per texel doesn't work.</t>
         </r>
@@ -2195,7 +2022,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Render a black screen</t>
         </r>
@@ -2237,7 +2064,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Clearing a FBO bigger than the window dimentions generate unclear bands</t>
         </r>
@@ -2265,7 +2092,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">glClearBufferfv is always performed, even is the condition fails.
 OpenGL 4.3 - 10.10 Conditional Rendering:
@@ -2325,7 +2152,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>"The internal format of the texture arrays is integer (see table 3.12), and either the magniﬁcation ﬁlter is not NEAREST, or the miniﬁcation ﬁlter is neither NEAREST nor NEAREST_MIPMAP_NEAREST."
 Other implementation doesn't have this requirement</t>
@@ -2564,7 +2391,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Fixed with the new drivers</t>
         </r>
@@ -2620,7 +2447,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Fixed in this drivers</t>
         </r>
@@ -2634,7 +2461,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">The implementation is confusing block name and instance name when enumerating uniforms
 </t>
@@ -2677,7 +2504,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">The depth test can't be enable
 </t>
@@ -2692,7 +2519,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">The depth test can't be enable
 </t>
@@ -2721,7 +2548,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Clearing a FBO failed</t>
         </r>
@@ -2735,7 +2562,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Generates a GL_FRAMEBUFFER_INCOMPLETE_DRAW_BUFFER error
 </t>
@@ -2750,7 +2577,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Generates a GL_FRAMEBUFFER_INCOMPLETE_DRAW_BUFFER error
 </t>
@@ -2765,7 +2592,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Fixed with this new driver</t>
         </r>
@@ -2807,7 +2634,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Blit of integer multisample texture with even a single sample per texel doesn't work.</t>
         </r>
@@ -2821,7 +2648,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Blit of integer multisample texture with even a single sample per texel doesn't work.</t>
         </r>
@@ -2835,7 +2662,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Render a black screen</t>
         </r>
@@ -2877,7 +2704,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Clearing a FBO bigger than the window dimentions generate unclear bands</t>
         </r>
@@ -2905,7 +2732,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">glClearBufferfv is always performed, even is the condition fails.
 OpenGL 4.3 - 10.10 Conditional Rendering:
@@ -2965,7 +2792,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>"The internal format of the texture arrays is integer (see table 3.12), and either the magniﬁcation ﬁlter is not NEAREST, or the miniﬁcation ﬁlter is neither NEAREST nor NEAREST_MIPMAP_NEAREST."
 Other implementation doesn't have this requirement</t>
@@ -3162,7 +2989,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Fixed with the new drivers</t>
         </r>
@@ -3218,7 +3045,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">The implementation is confusing block name and instance name when enumerating uniforms
 </t>
@@ -3233,7 +3060,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">The implementation is confusing block name and instance name when enumerating uniforms
 </t>
@@ -3276,7 +3103,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">The depth test can't be enable
 </t>
@@ -3291,7 +3118,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">The depth test can't be enable
 </t>
@@ -3320,7 +3147,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Clearing a FBO failed</t>
         </r>
@@ -3334,7 +3161,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Crash when there is only a depth attachment
 </t>
@@ -3349,7 +3176,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Generates a GL_FRAMEBUFFER_INCOMPLETE_DRAW_BUFFER error
 </t>
@@ -3364,7 +3191,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Fixed with this new driver</t>
         </r>
@@ -3406,7 +3233,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Blit of integer multisample texture with even a single sample per texel doesn't work.</t>
         </r>
@@ -3420,7 +3247,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Blit of integer multisample texture with even a single sample per texel doesn't work.</t>
         </r>
@@ -3434,7 +3261,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Render a black screen</t>
         </r>
@@ -3476,7 +3303,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Clearing a FBO bigger than the window dimentions generate unclear bands</t>
         </r>
@@ -3490,7 +3317,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>No error but doesn't render anything</t>
         </r>
@@ -3518,7 +3345,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">glClearBufferfv is always performed, even is the condition fails.
 OpenGL 4.3 - 10.10 Conditional Rendering:
@@ -3578,7 +3405,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>"The internal format of the texture arrays is integer (see table 3.12), and either the magniﬁcation ﬁlter is not NEAREST, or the miniﬁcation ﬁlter is neither NEAREST nor NEAREST_MIPMAP_NEAREST."
 Other implementation doesn't have this requirement</t>
@@ -3775,7 +3602,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Fixed with the new drivers</t>
         </r>
@@ -3831,7 +3658,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">The implementation is confusing block name and instance name when enumerating uniforms
 </t>
@@ -3846,7 +3673,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">The implementation is confusing block name and instance name when enumerating uniforms
 </t>
@@ -3861,7 +3688,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Can't use the layout qualifier at a glocal scope on uniforms. Generate a GLSL compiler error.</t>
         </r>
@@ -3889,7 +3716,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">The depth test can't be enable
 </t>
@@ -3904,7 +3731,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">The depth test can't be enable
 </t>
@@ -3933,7 +3760,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Clearing a FBO failed</t>
         </r>
@@ -3947,7 +3774,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Crash when there is only a depth attachment
 </t>
@@ -3962,7 +3789,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Generates a GL_FRAMEBUFFER_INCOMPLETE_DRAW_BUFFER error
 </t>
@@ -3977,7 +3804,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Fixed with this new driver</t>
         </r>
@@ -4019,7 +3846,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Blit of integer multisample texture with even a single sample per texel doesn't work.</t>
         </r>
@@ -4033,7 +3860,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Blit of integer multisample texture with even a single sample per texel doesn't work.</t>
         </r>
@@ -4047,7 +3874,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Render a black screen</t>
         </r>
@@ -4089,7 +3916,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Clearing a FBO bigger than the window dimentions generate unclear bands</t>
         </r>
@@ -4103,7 +3930,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Doesn't allow to redeclare any built-in blocks in any shader stage</t>
         </r>
@@ -4117,7 +3944,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Generates a GLSL error: unknown opcode modifier
 </t>
@@ -4132,7 +3959,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Compiler crash</t>
         </r>
@@ -4160,7 +3987,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">glClearBufferfv is always performed, even is the condition fails.
 OpenGL 4.3 - 10.10 Conditional Rendering:
@@ -4206,7 +4033,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Deleting shader object after being attached lead to invalid operations error generated when the program pop the stack</t>
         </r>
@@ -4234,7 +4061,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>"The internal format of the texture arrays is integer (see table 3.12), and either the magniﬁcation ﬁlter is not NEAREST, or the miniﬁcation ﬁlter is neither NEAREST nor NEAREST_MIPMAP_NEAREST."
 Other implementation doesn't have this requirement</t>
@@ -4835,7 +4662,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Crash when there is only a depth attachment
 </t>
@@ -4850,7 +4677,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Generates a GL_FRAMEBUFFER_INCOMPLETE_DRAW_BUFFER error
 </t>
@@ -4865,7 +4692,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Crash
 </t>
@@ -6016,7 +5843,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7181" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7183" uniqueCount="371">
   <si>
     <t>gl-430-texture-view</t>
   </si>
@@ -7077,9 +6904,6 @@
     <t>OpenGL Status - February 2014</t>
   </si>
   <si>
-    <t>4.4.1.2</t>
-  </si>
-  <si>
     <t>OpenGL ES 3.0</t>
   </si>
   <si>
@@ -7110,13 +6934,28 @@
     <t>430-perf-monitor-amd</t>
   </si>
   <si>
-    <t>02/18/2013</t>
-  </si>
-  <si>
     <t>334.89</t>
   </si>
   <si>
     <t>NVIDIA 334.89</t>
+  </si>
+  <si>
+    <t>10.18.10.3380</t>
+  </si>
+  <si>
+    <t>Intel 10.18.10.3380</t>
+  </si>
+  <si>
+    <t>14.1 beta 1</t>
+  </si>
+  <si>
+    <t>AMD 14.1 beta 1</t>
+  </si>
+  <si>
+    <t>10/22/2013</t>
+  </si>
+  <si>
+    <t>4.4.1.3</t>
   </si>
 </sst>
 </file>
@@ -7126,7 +6965,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7189,13 +7028,6 @@
       <name val="Cambria"/>
       <family val="1"/>
       <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -7454,6 +7286,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7474,9 +7309,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -7585,10 +7417,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.83333333333333337</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8666666666666667</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -7597,7 +7429,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.95</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
@@ -7618,7 +7450,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AMD 13.11 b9.2</c:v>
+                  <c:v>AMD 14.1 beta 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7679,7 +7511,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.9</c:v>
+                  <c:v>0.95</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.91666666666666663</c:v>
@@ -7700,7 +7532,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Intel 10.18.10.3325</c:v>
+                  <c:v>Intel 10.18.10.3380</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7758,7 +7590,7 @@
                   <c:v>0.83333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.8571428571428571</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.95</c:v>
@@ -7840,16 +7672,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.42857142857142855</c:v>
+                  <c:v>0.5714285714285714</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.7</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.91666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.90196078431372551</c:v>
+                  <c:v>0.92307692307692313</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7864,11 +7696,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="148280832"/>
-        <c:axId val="148128320"/>
+        <c:axId val="148780032"/>
+        <c:axId val="148660224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="148280832"/>
+        <c:axId val="148780032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7877,7 +7709,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148128320"/>
+        <c:crossAx val="148660224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7885,7 +7717,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="148128320"/>
+        <c:axId val="148660224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -7897,7 +7729,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148280832"/>
+        <c:crossAx val="148780032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8277,11 +8109,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="143762944"/>
-        <c:axId val="148131200"/>
+        <c:axId val="151285760"/>
+        <c:axId val="148663104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="143762944"/>
+        <c:axId val="151285760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8290,7 +8122,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148131200"/>
+        <c:crossAx val="148663104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8298,7 +8130,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="148131200"/>
+        <c:axId val="148663104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -8310,13 +8142,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143762944"/>
+        <c:crossAx val="151285760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8689,11 +8522,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="149567488"/>
-        <c:axId val="148134656"/>
+        <c:axId val="151289344"/>
+        <c:axId val="148665984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="149567488"/>
+        <c:axId val="151289344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8702,7 +8535,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148134656"/>
+        <c:crossAx val="148665984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8710,7 +8543,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="148134656"/>
+        <c:axId val="148665984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -8722,7 +8555,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149567488"/>
+        <c:crossAx val="151289344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9077,11 +8910,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="149565440"/>
-        <c:axId val="149734528"/>
+        <c:axId val="151693312"/>
+        <c:axId val="151176320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="149565440"/>
+        <c:axId val="151693312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9090,7 +8923,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149734528"/>
+        <c:crossAx val="151176320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9098,7 +8931,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="149734528"/>
+        <c:axId val="151176320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -9110,7 +8943,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149565440"/>
+        <c:crossAx val="151693312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9465,11 +9298,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="150687232"/>
-        <c:axId val="149737408"/>
+        <c:axId val="151955968"/>
+        <c:axId val="151178624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="150687232"/>
+        <c:axId val="151955968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9478,7 +9311,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149737408"/>
+        <c:crossAx val="151178624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9486,7 +9319,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="149737408"/>
+        <c:axId val="151178624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -9498,7 +9331,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150687232"/>
+        <c:crossAx val="151955968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9853,11 +9686,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="151726080"/>
-        <c:axId val="149740288"/>
+        <c:axId val="152207360"/>
+        <c:axId val="151181504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="151726080"/>
+        <c:axId val="152207360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9866,7 +9699,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149740288"/>
+        <c:crossAx val="151181504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9874,7 +9707,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="149740288"/>
+        <c:axId val="151181504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -9886,7 +9719,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151726080"/>
+        <c:crossAx val="152207360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10393,11 +10226,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="143761920"/>
-        <c:axId val="150906560"/>
+        <c:axId val="152162304"/>
+        <c:axId val="151839296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="143761920"/>
+        <c:axId val="152162304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10406,7 +10239,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150906560"/>
+        <c:crossAx val="151839296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10414,7 +10247,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="150906560"/>
+        <c:axId val="151839296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -10426,7 +10259,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143761920"/>
+        <c:crossAx val="152162304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10897,11 +10730,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="150582784"/>
-        <c:axId val="150908864"/>
+        <c:axId val="143360512"/>
+        <c:axId val="151841600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="150582784"/>
+        <c:axId val="143360512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10910,7 +10743,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150908864"/>
+        <c:crossAx val="151841600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10918,7 +10751,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="150908864"/>
+        <c:axId val="151841600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -10930,7 +10763,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150582784"/>
+        <c:crossAx val="143360512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10956,15 +10789,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>138111</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:colOff>176211</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>790575</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>828675</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11532,8 +11365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="F213" sqref="F213"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11547,22 +11380,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="61" t="s">
         <v>352</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="62" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
@@ -11592,17 +11425,17 @@
       <c r="A5" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B5" s="17" t="s">
-        <v>364</v>
+      <c r="B5" s="17">
+        <v>41688</v>
       </c>
       <c r="C5" s="17">
-        <v>41586</v>
+        <v>41671</v>
       </c>
       <c r="D5" s="39">
-        <v>41516</v>
-      </c>
-      <c r="E5" s="17">
-        <v>41569</v>
+        <v>41683</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -11610,13 +11443,13 @@
         <v>148</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="D6" s="57" t="s">
         <v>365</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="D6" s="57" t="s">
-        <v>348</v>
       </c>
       <c r="E6" s="23" t="s">
         <v>341</v>
@@ -11627,16 +11460,16 @@
         <v>157</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>353</v>
+        <v>370</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>353</v>
+        <v>370</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>353</v>
+        <v>370</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>353</v>
+        <v>370</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11651,13 +11484,13 @@
         <v>161</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>366</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>347</v>
       </c>
       <c r="E9" s="27" t="s">
         <v>341</v>
@@ -11669,7 +11502,7 @@
       </c>
       <c r="B10" s="49">
         <f>IF(B$48=0, 0,(B$43+B$44)/B$48)</f>
-        <v>0.83333333333333337</v>
+        <v>1</v>
       </c>
       <c r="C10" s="49">
         <f t="shared" ref="C10:E10" si="0">IF(C$48=0, 0,(C$43+C$44)/C$48)</f>
@@ -11690,7 +11523,7 @@
       </c>
       <c r="B11" s="20">
         <f>IF(B$72=0, 0,(B$67+B$68)/B$72)</f>
-        <v>0.8666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C11" s="20">
         <f>IF(C$72=0, 0,(C$67+C$68)/C$72)</f>
@@ -11740,11 +11573,11 @@
       </c>
       <c r="D13" s="20">
         <f>IF(D$121=0, 0, (D$116+D$117)/D$121)</f>
-        <v>0.8571428571428571</v>
+        <v>1</v>
       </c>
       <c r="E13" s="20">
         <f>IF(E$121=0, 0, (E$116+E$117)/E$121)</f>
-        <v>0.42857142857142855</v>
+        <v>0.5714285714285714</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -11753,11 +11586,11 @@
       </c>
       <c r="B14" s="20">
         <f>IF(B$150=0, 0, (B$145+B$146)/B$150)</f>
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="C14" s="20">
         <f>IF(C$150=0, 0, (C$145+C$146)/C$150)</f>
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="D14" s="20">
         <f>IF(D$150=0, 0, (D$145+D$146)/D$150)</f>
@@ -11765,7 +11598,7 @@
       </c>
       <c r="E14" s="20">
         <f>IF(E$150=0, 0, (E$145+E$146)/E$150)</f>
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -11807,7 +11640,7 @@
       </c>
       <c r="E16" s="25">
         <f>IF(E$233=0, 0, (E$228+E$229)/E$233)</f>
-        <v>0.90196078431372551</v>
+        <v>0.92307692307692313</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -11996,8 +11829,8 @@
       <c r="A39" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B39" s="8" t="s">
-        <v>7</v>
+      <c r="B39" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="C39" s="57" t="s">
         <v>177</v>
@@ -12066,7 +11899,7 @@
       </c>
       <c r="B43" s="10">
         <f>COUNTIF(B37:B42,"pass")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C43" s="10">
         <f>COUNTIF(C37:C42,"pass")</f>
@@ -12129,7 +11962,7 @@
       </c>
       <c r="B46" s="12">
         <f>COUNTIF(B37:B42,"Fail")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C46" s="12">
         <f>COUNTIF(C37:C42,"Fail")</f>
@@ -12192,7 +12025,7 @@
       </c>
       <c r="B49" s="6">
         <f>IF(B$48=0, 0,(B$43+B$44)/B$48)</f>
-        <v>0.83333333333333337</v>
+        <v>1</v>
       </c>
       <c r="C49" s="6">
         <f t="shared" ref="C49:E49" si="1">IF(C$48=0, 0,(C$43+C$44)/C$48)</f>
@@ -12250,8 +12083,8 @@
       <c r="A53" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B53" s="7" t="s">
-        <v>140</v>
+      <c r="B53" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>7</v>
@@ -12335,8 +12168,8 @@
       <c r="A58" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B58" s="7" t="s">
-        <v>140</v>
+      <c r="B58" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>6</v>
@@ -12474,7 +12307,7 @@
       <c r="B66" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C66" s="67" t="s">
+      <c r="C66" s="60" t="s">
         <v>7</v>
       </c>
       <c r="D66" s="31" t="s">
@@ -12490,7 +12323,7 @@
       </c>
       <c r="B67" s="10">
         <f>COUNTIF(B52:B66,"pass")</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C67" s="10">
         <f>COUNTIF(C52:C66,"pass")</f>
@@ -12532,7 +12365,7 @@
       </c>
       <c r="B69" s="11">
         <f>COUNTIF(B52:B66,"workaround")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C69" s="11">
         <f>COUNTIF(C52:C66,"workaround")</f>
@@ -12616,7 +12449,7 @@
       </c>
       <c r="B73" s="6">
         <f>IF(B$72=0, 0,(B$67+B$68)/B$72)</f>
-        <v>0.8666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C73" s="6">
         <f>IF(C$72=0, 0,(C$67+C$68)/C$72)</f>
@@ -12829,8 +12662,8 @@
       <c r="A86" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B86" s="35" t="s">
-        <v>144</v>
+      <c r="B86" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="C86" s="4" t="s">
         <v>6</v>
@@ -13069,7 +12902,7 @@
       </c>
       <c r="B100" s="10">
         <f>COUNTIF(B76:B99,"pass")</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C100" s="10">
         <f>COUNTIF(C76:C99,"pass")</f>
@@ -13090,7 +12923,7 @@
       </c>
       <c r="B101" s="5">
         <f>COUNTIF(B76:B99,"Ok")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C101" s="5">
         <f>COUNTIF(C76:C99,"Ok")</f>
@@ -13264,8 +13097,8 @@
       <c r="D110" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E110" s="8" t="s">
-        <v>7</v>
+      <c r="E110" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -13329,11 +13162,11 @@
       <c r="C114" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D114" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E114" s="4" t="s">
-        <v>6</v>
+      <c r="D114" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E114" s="35" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -13367,7 +13200,7 @@
       </c>
       <c r="D116" s="10">
         <f>COUNTIF(D109:D115,"pass")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E116" s="10">
         <f>COUNTIF(E109:E115,"pass")</f>
@@ -13392,7 +13225,7 @@
       </c>
       <c r="E117" s="5">
         <f>COUNTIF(E109:E115,"Ok")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -13430,11 +13263,11 @@
       </c>
       <c r="D119" s="12">
         <f>COUNTIF(D109:D115,"Fail")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E119" s="12">
         <f>COUNTIF(E109:E115,"Fail")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -13493,11 +13326,11 @@
       </c>
       <c r="D122" s="6">
         <f>IF(D$121=0, 0, (D$116+D$117)/D$121)</f>
-        <v>0.8571428571428571</v>
+        <v>1</v>
       </c>
       <c r="E122" s="6">
         <f>IF(E$121=0, 0, (E$116+E$117)/E$121)</f>
-        <v>0.42857142857142855</v>
+        <v>0.5714285714285714</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13537,8 +13370,8 @@
       <c r="D125" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E125" s="4" t="s">
-        <v>6</v>
+      <c r="E125" s="8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -13656,8 +13489,8 @@
       <c r="D132" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E132" s="8" t="s">
-        <v>7</v>
+      <c r="E132" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -13792,8 +13625,8 @@
       <c r="D140" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E140" s="8" t="s">
-        <v>7</v>
+      <c r="E140" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -13826,8 +13659,8 @@
       <c r="D142" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E142" s="35" t="s">
-        <v>144</v>
+      <c r="E142" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -13851,11 +13684,11 @@
       <c r="A144" s="15" t="s">
         <v>277</v>
       </c>
-      <c r="B144" s="22" t="s">
-        <v>140</v>
-      </c>
-      <c r="C144" s="22" t="s">
-        <v>140</v>
+      <c r="B144" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C144" s="21" t="s">
+        <v>6</v>
       </c>
       <c r="D144" s="21" t="s">
         <v>6</v>
@@ -13870,11 +13703,11 @@
       </c>
       <c r="B145" s="10">
         <f>COUNTIF(B125:B144,"pass")</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C145" s="10">
         <f>COUNTIF(C125:C144,"pass")</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D145" s="10">
         <f>COUNTIF(D125:D144,"pass")</f>
@@ -13882,7 +13715,7 @@
       </c>
       <c r="E145" s="10">
         <f>COUNTIF(E125:E144,"pass")</f>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -13903,7 +13736,7 @@
       </c>
       <c r="E146" s="5">
         <f>COUNTIF(E125:E144,"Ok")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -13912,11 +13745,11 @@
       </c>
       <c r="B147" s="11">
         <f>COUNTIF(B125:B144,"workaround")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C147" s="11">
         <f>COUNTIF(C125:C144,"workaround")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D147" s="11">
         <f>COUNTIF(D125:D144,"workaround")</f>
@@ -13945,7 +13778,7 @@
       </c>
       <c r="E148" s="12">
         <f>COUNTIF(E125:E144,"Fail")</f>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -13996,11 +13829,11 @@
       </c>
       <c r="B151" s="6">
         <f>IF(B$150=0, 0, (B$145+B$146)/B$150)</f>
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="C151" s="6">
         <f>IF(C$150=0, 0, (C$145+C$146)/C$150)</f>
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="D151" s="6">
         <f>IF(D$150=0, 0, (D$145+D$146)/D$150)</f>
@@ -14008,7 +13841,7 @@
       </c>
       <c r="E151" s="6">
         <f>IF(E$150=0, 0, (E$145+E$146)/E$150)</f>
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14065,8 +13898,8 @@
       <c r="D155" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E155" s="4" t="s">
-        <v>6</v>
+      <c r="E155" s="8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -14201,8 +14034,8 @@
       <c r="D163" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E163" s="8" t="s">
-        <v>7</v>
+      <c r="E163" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -14531,7 +14364,7 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B182" s="4" t="s">
         <v>6</v>
@@ -14548,7 +14381,7 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B183" s="4" t="s">
         <v>6</v>
@@ -14780,8 +14613,8 @@
       <c r="D196" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E196" s="53" t="s">
-        <v>7</v>
+      <c r="E196" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
@@ -14803,7 +14636,7 @@
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="23" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B198" s="8" t="s">
         <v>7</v>
@@ -14814,8 +14647,8 @@
       <c r="D198" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E198" s="4" t="s">
-        <v>6</v>
+      <c r="E198" s="8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
@@ -14854,7 +14687,7 @@
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B201" s="8" t="s">
         <v>7</v>
@@ -14933,6 +14766,9 @@
       <c r="D205" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="E205" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
@@ -14981,13 +14817,13 @@
       <c r="D208" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E208" s="53" t="s">
-        <v>7</v>
+      <c r="E208" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="23" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B209" s="4" t="s">
         <v>6</v>
@@ -15326,7 +15162,7 @@
       </c>
       <c r="E228" s="10">
         <f>COUNTIF(E$176:E$227,"pass")</f>
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
@@ -15389,7 +15225,7 @@
       </c>
       <c r="E231" s="12">
         <f>COUNTIF(E176:E227,"Fail")</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
@@ -15431,7 +15267,7 @@
       </c>
       <c r="E233" s="2">
         <f>E$228+E$231+E$230+E$232+E$229</f>
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="234" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15452,7 +15288,7 @@
       </c>
       <c r="E234" s="6">
         <f>IF(E$233=0, 0, (E$228+E$229)/E$233)</f>
-        <v>0.90196078431372551</v>
+        <v>0.92307692307692313</v>
       </c>
     </row>
     <row r="235" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15481,7 +15317,7 @@
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B237" s="2"/>
       <c r="C237" s="4" t="s">
@@ -15497,7 +15333,9 @@
       <c r="B238" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C238" s="2"/>
+      <c r="C238" s="8" t="s">
+        <v>7</v>
+      </c>
       <c r="D238" s="2"/>
       <c r="E238" s="2"/>
     </row>
@@ -15650,7 +15488,7 @@
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B252" s="4" t="s">
         <v>6</v>
@@ -15678,7 +15516,7 @@
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B254" s="4" t="s">
         <v>6</v>
@@ -15764,7 +15602,7 @@
       </c>
       <c r="C258" s="12">
         <f t="shared" ref="C258:E258" si="5">COUNTIF(C237:C254,"Fail")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D258" s="12">
         <f t="shared" si="5"/>
@@ -15806,7 +15644,7 @@
       </c>
       <c r="C260" s="2">
         <f>C255+C258+C257+C259+C256</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D260" s="2">
         <f>D255+D258+D257+D259+D256</f>
@@ -15827,7 +15665,7 @@
       </c>
       <c r="C261" s="6">
         <f>IF(C$260=0, 0, (C$255+C$256)/C$260)</f>
-        <v>1</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="D261" s="6">
         <f>IF(D$260=0, 0, (D$255+D$256)/D$260)</f>
@@ -15847,7 +15685,7 @@
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="15" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B263" s="15"/>
       <c r="C263" s="15"/>
@@ -15856,7 +15694,7 @@
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="28" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B264" s="29" t="s">
         <v>6</v>
@@ -16237,7 +16075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E260"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
+    <sheetView topLeftCell="A172" workbookViewId="0">
       <selection activeCell="I122" sqref="I122"/>
     </sheetView>
   </sheetViews>
@@ -16252,22 +16090,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="61" t="s">
         <v>345</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="62" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
@@ -20545,22 +20383,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="61" t="s">
         <v>332</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="62" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
@@ -24821,22 +24659,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="61" t="s">
         <v>330</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="62" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
@@ -28820,22 +28658,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="61" t="s">
         <v>318</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="62" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
@@ -32819,22 +32657,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="61" t="s">
         <v>197</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="62" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
@@ -36819,26 +36657,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="61" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="62" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
@@ -36853,18 +36691,18 @@
       <c r="A4" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="63"/>
-      <c r="D4" s="64" t="s">
+      <c r="C4" s="64"/>
+      <c r="D4" s="65" t="s">
         <v>151</v>
       </c>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64" t="s">
+      <c r="E4" s="65"/>
+      <c r="F4" s="65" t="s">
         <v>150</v>
       </c>
-      <c r="G4" s="64"/>
+      <c r="G4" s="65"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -42166,26 +42004,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="62" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
@@ -42200,18 +42038,18 @@
       <c r="A4" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="63"/>
-      <c r="D4" s="64" t="s">
+      <c r="C4" s="64"/>
+      <c r="D4" s="65" t="s">
         <v>151</v>
       </c>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64" t="s">
+      <c r="E4" s="65"/>
+      <c r="F4" s="65" t="s">
         <v>150</v>
       </c>
-      <c r="G4" s="64"/>
+      <c r="G4" s="65"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -46872,14 +46710,14 @@
       <c r="A1" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="66" t="s">
+      <c r="C1" s="66"/>
+      <c r="D1" s="67" t="s">
         <v>151</v>
       </c>
-      <c r="E1" s="66"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">

</xml_diff>